<commit_message>
Included new version of kinetic theory lab in spreadsheet
This is a version of the kinetic theory lab that I (Matt) wrote in spring 2020 during COVID, which does not use simulation software.  It has both advantages and disadvantages w.r.t. the original kinetic theory lab.  Maybe someday someone can recombine the two versions to get the best of both worlds.  For now, I include it here as an option in the master.tex files and the spreadsheet.
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2021spring.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2021spring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Desktop\github\132\StudentGuideModule2\what_labs_to_include\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D0F31E-C682-4224-955E-AD32C4C4C8F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747CCA84-CDAC-4184-B909-705275FD06F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18780" yWindow="5136" windowWidth="26616" windowHeight="15936" tabRatio="541" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -884,7 +884,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P62" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
+    <comment ref="P63" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
       <text>
         <r>
           <rPr>
@@ -909,7 +909,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P65" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
+    <comment ref="P66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
       <text>
         <r>
           <rPr>
@@ -933,7 +933,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P68" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
+    <comment ref="P69" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
       <text>
         <r>
           <rPr>
@@ -958,7 +958,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P75" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
+    <comment ref="P76" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
       <text>
         <r>
           <rPr>
@@ -987,7 +987,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="242">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -1573,9 +1573,6 @@
     <t>Not updated for Capstone</t>
   </si>
   <si>
-    <t>2018 spr Ovidiu</t>
-  </si>
-  <si>
     <t>Using 32-bit applications in Windows</t>
   </si>
   <si>
@@ -1648,9 +1645,6 @@
     <t>Force by Editor</t>
   </si>
   <si>
-    <t>2020 spr Jerry</t>
-  </si>
-  <si>
     <t>2019 fall Christine</t>
   </si>
   <si>
@@ -1676,9 +1670,6 @@
   </si>
   <si>
     <t>Needed for kinetic theory labs?</t>
-  </si>
-  <si>
-    <t>2020 fall Jack</t>
   </si>
   <si>
     <t>2020 fall Matt</t>
@@ -1710,6 +1701,21 @@
   </si>
   <si>
     <t>Heat of Vaporization of Nitrogen [prescriptive version]</t>
+  </si>
+  <si>
+    <t>Kinetic Theory of Ideal Gases, and Equipartition of Energy</t>
+  </si>
+  <si>
+    <t>2021 spr Ovidiu</t>
+  </si>
+  <si>
+    <t>2021 spr Jerry</t>
+  </si>
+  <si>
+    <t>2021 spr Jack</t>
+  </si>
+  <si>
+    <t>no-software version by MT, 2020</t>
   </si>
 </sst>
 </file>
@@ -2913,11 +2919,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD121"/>
+  <dimension ref="A1:AD122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2948,7 +2954,7 @@
         <v>107</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D1" s="48" t="s">
         <v>85</v>
@@ -2957,7 +2963,7 @@
         <v>86</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G1" s="48" t="s">
         <v>175</v>
@@ -2978,31 +2984,31 @@
         <v>100</v>
       </c>
       <c r="M1" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="N1" s="47" t="s">
         <v>210</v>
       </c>
-      <c r="N1" s="47" t="s">
-        <v>211</v>
-      </c>
       <c r="O1" s="47" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="P1" s="47" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="Q1" s="47" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="R1" s="47" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="S1" s="47" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="T1" s="47" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U1" s="50" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="V1" s="30"/>
       <c r="W1" s="31"/>
@@ -3029,7 +3035,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="54">
-        <f>CEILING(D2,W$22+1)</f>
+        <f t="shared" ref="F2:F33" si="0">CEILING(D2,W$22+1)</f>
         <v>4</v>
       </c>
       <c r="G2" s="54"/>
@@ -3055,7 +3061,7 @@
         <v>2</v>
       </c>
       <c r="U2" s="67">
-        <f>SUM(R2:T2)</f>
+        <f>SUM(Q2:T2)</f>
         <v>4</v>
       </c>
       <c r="V2" s="31"/>
@@ -3081,7 +3087,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="58">
-        <f>CEILING(D3,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G3" s="58"/>
@@ -3107,7 +3113,7 @@
         <v>2</v>
       </c>
       <c r="U3" s="81">
-        <f>SUM(R3:T3)</f>
+        <f t="shared" ref="U3:U66" si="1">SUM(Q3:T3)</f>
         <v>4</v>
       </c>
       <c r="V3" s="31"/>
@@ -3128,7 +3134,7 @@
         <v>110</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D4" s="13">
         <v>5</v>
@@ -3137,7 +3143,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="13">
-        <f>CEILING(D4,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G4" s="13">
@@ -3179,8 +3185,8 @@
       </c>
       <c r="T4" s="77"/>
       <c r="U4" s="67">
-        <f>SUM(R4:T4)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="V4" s="31"/>
       <c r="W4" s="5"/>
@@ -3197,7 +3203,7 @@
         <v>155</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D5" s="13">
         <v>2</v>
@@ -3206,7 +3212,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="13">
-        <f>CEILING(D5,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G5" s="13">
@@ -3244,8 +3250,8 @@
         <v>1</v>
       </c>
       <c r="U5" s="67">
-        <f>SUM(R5:T5)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="V5" s="31"/>
       <c r="W5" s="5"/>
@@ -3263,7 +3269,7 @@
         <v>156</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D6" s="13">
         <v>2</v>
@@ -3272,7 +3278,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="13">
-        <f>CEILING(D6,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H6" s="13">
@@ -3300,7 +3306,7 @@
       <c r="S6" s="77"/>
       <c r="T6" s="77"/>
       <c r="U6" s="67">
-        <f>SUM(R6:T6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V6" s="31"/>
@@ -3319,7 +3325,7 @@
         <v>179</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D7" s="26">
         <v>1</v>
@@ -3328,7 +3334,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="26">
-        <f>CEILING(D7,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G7" s="26"/>
@@ -3350,7 +3356,7 @@
       <c r="S7" s="78"/>
       <c r="T7" s="78"/>
       <c r="U7" s="81">
-        <f>SUM(R7:T7)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W7" s="5"/>
@@ -3366,7 +3372,7 @@
         <v>171</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D8" s="13">
         <v>4</v>
@@ -3375,7 +3381,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="13">
-        <f>CEILING(D8,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I8" s="13">
@@ -3409,8 +3415,8 @@
         <v>1</v>
       </c>
       <c r="U8" s="67">
-        <f>SUM(R8:T8)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="V8" s="31"/>
       <c r="W8" s="5"/>
@@ -3427,7 +3433,7 @@
         <v>111</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D9" s="13">
         <v>2</v>
@@ -3436,7 +3442,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="13">
-        <f>CEILING(D9,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H9" s="13">
@@ -3470,8 +3476,8 @@
         <v>1</v>
       </c>
       <c r="U9" s="67">
-        <f>SUM(R9:T9)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="V9" s="31"/>
       <c r="W9" s="5"/>
@@ -3488,7 +3494,7 @@
         <v>112</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D10" s="13">
         <v>5</v>
@@ -3497,7 +3503,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="13">
-        <f>CEILING(D10,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G10" s="13">
@@ -3519,7 +3525,7 @@
         <v>0.5</v>
       </c>
       <c r="U10" s="67">
-        <f>SUM(R10:T10)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="V10" s="31"/>
@@ -3537,7 +3543,7 @@
         <v>113</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D11" s="13">
         <v>2</v>
@@ -3546,7 +3552,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="13">
-        <f>CEILING(D11,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H11" s="13">
@@ -3580,8 +3586,8 @@
         <v>1</v>
       </c>
       <c r="U11" s="67">
-        <f>SUM(R11:T11)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="V11" s="31"/>
       <c r="W11" s="40" t="s">
@@ -3597,10 +3603,10 @@
     </row>
     <row r="12" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="22" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D12" s="13">
         <v>4</v>
@@ -3609,11 +3615,11 @@
         <v>1</v>
       </c>
       <c r="F12" s="13">
-        <f>CEILING(D12,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L12" s="75"/>
       <c r="P12" s="77">
@@ -3627,7 +3633,7 @@
         <v>1</v>
       </c>
       <c r="U12" s="67">
-        <f>SUM(R12:T12)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V12" s="31"/>
@@ -3644,10 +3650,10 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13" s="13">
         <v>3</v>
@@ -3656,11 +3662,11 @@
         <v>0</v>
       </c>
       <c r="F13" s="13">
-        <f>CEILING(D13,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L13" s="75"/>
       <c r="P13" s="77">
@@ -3674,7 +3680,7 @@
         <v>1</v>
       </c>
       <c r="U13" s="67">
-        <f>SUM(R13:T13)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V13" s="31"/>
@@ -3689,10 +3695,10 @@
     </row>
     <row r="14" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="22" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D14" s="13">
         <v>3</v>
@@ -3701,17 +3707,17 @@
         <v>0</v>
       </c>
       <c r="F14" s="13">
-        <f>CEILING(D14,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L14" s="75"/>
       <c r="P14" s="77"/>
       <c r="Q14" s="75"/>
       <c r="U14" s="67">
-        <f>SUM(R14:T14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V14" s="31"/>
@@ -3727,10 +3733,10 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D15" s="13">
         <v>3</v>
@@ -3739,17 +3745,17 @@
         <v>0</v>
       </c>
       <c r="F15" s="13">
-        <f>CEILING(D15,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L15" s="75"/>
       <c r="P15" s="77"/>
       <c r="Q15" s="75"/>
       <c r="U15" s="67">
-        <f>SUM(R15:T15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V15" s="31"/>
@@ -3771,7 +3777,7 @@
         <v>181</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D16" s="13">
         <v>9</v>
@@ -3780,7 +3786,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="13">
-        <f>CEILING(D16,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K16" s="21" t="s">
@@ -3811,8 +3817,8 @@
         <v>1</v>
       </c>
       <c r="U16" s="67">
-        <f>SUM(R16:T16)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="V16" s="31"/>
       <c r="W16" s="17" t="s">
@@ -3833,7 +3839,7 @@
         <v>184</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D17" s="13">
         <v>3</v>
@@ -3842,7 +3848,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="13">
-        <f>CEILING(D17,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G17" s="13">
@@ -3883,8 +3889,8 @@
         <v>1</v>
       </c>
       <c r="U17" s="67">
-        <f>SUM(R17:T17)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="V17" s="31"/>
       <c r="W17" s="17" t="s">
@@ -3905,7 +3911,7 @@
         <v>182</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D18" s="13">
         <v>5</v>
@@ -3914,7 +3920,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="13">
-        <f>CEILING(D18,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="K18" s="21" t="s">
@@ -3939,8 +3945,8 @@
         <v>1</v>
       </c>
       <c r="U18" s="67">
-        <f>SUM(R18:T18)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="V18" s="31"/>
       <c r="W18" s="17" t="s">
@@ -3961,7 +3967,7 @@
         <v>183</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D19" s="13">
         <v>4</v>
@@ -3970,7 +3976,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="13">
-        <f>CEILING(D19,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K19" s="21" t="s">
@@ -4001,8 +4007,8 @@
         <v>0.1</v>
       </c>
       <c r="U19" s="67">
-        <f>SUM(R19:T19)</f>
-        <v>1.1000000000000001</v>
+        <f t="shared" si="1"/>
+        <v>2.1</v>
       </c>
       <c r="V19" s="31"/>
       <c r="W19" s="18" t="s">
@@ -4023,7 +4029,7 @@
         <v>114</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D20" s="13">
         <v>5</v>
@@ -4032,7 +4038,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="13">
-        <f>CEILING(D20,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H20" s="13">
@@ -4066,8 +4072,8 @@
         <v>1</v>
       </c>
       <c r="U20" s="67">
-        <f>SUM(R20:T20)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="V20" s="31"/>
       <c r="Z20" s="31"/>
@@ -4081,7 +4087,7 @@
         <v>115</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D21" s="13">
         <v>3</v>
@@ -4090,7 +4096,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="13">
-        <f>CEILING(D21,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G21" s="13">
@@ -4101,12 +4107,12 @@
       <c r="P21" s="77"/>
       <c r="Q21" s="31"/>
       <c r="U21" s="67">
-        <f>SUM(R21:T21)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V21" s="31"/>
       <c r="W21" s="40" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X21" s="41"/>
       <c r="Y21" s="31"/>
@@ -4121,7 +4127,7 @@
         <v>116</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D22" s="13">
         <v>4</v>
@@ -4130,7 +4136,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="13">
-        <f>CEILING(D22,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G22" s="13">
@@ -4145,8 +4151,8 @@
         <v>1</v>
       </c>
       <c r="U22" s="67">
-        <f>SUM(R22:T22)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="V22" s="31"/>
       <c r="W22" s="42">
@@ -4165,7 +4171,7 @@
         <v>117</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D23" s="13">
         <v>2</v>
@@ -4174,7 +4180,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="13">
-        <f>CEILING(D23,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G23" s="13">
@@ -4202,7 +4208,7 @@
       </c>
       <c r="T23" s="78"/>
       <c r="U23" s="81">
-        <f>SUM(R23:T23)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V23" s="31"/>
@@ -4222,7 +4228,7 @@
         <v>118</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D24" s="12">
         <v>10</v>
@@ -4231,7 +4237,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="12">
-        <f>CEILING(D24,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G24" s="12"/>
@@ -4273,8 +4279,8 @@
       </c>
       <c r="T24" s="77"/>
       <c r="U24" s="67">
-        <f>SUM(R24:T24)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="V24" s="31"/>
       <c r="W24" s="14"/>
@@ -4289,7 +4295,7 @@
         <v>119</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D25" s="13">
         <v>8</v>
@@ -4298,7 +4304,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="13">
-        <f>CEILING(D25,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H25" s="13">
@@ -4338,8 +4344,8 @@
         <v>1</v>
       </c>
       <c r="U25" s="67">
-        <f>SUM(R25:T25)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="V25" s="31"/>
       <c r="W25" s="44" t="s">
@@ -4361,10 +4367,10 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D26" s="13">
         <v>3</v>
@@ -4373,11 +4379,11 @@
         <v>0</v>
       </c>
       <c r="F26" s="13">
-        <f>CEILING(D26,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K26" s="21" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L26" s="75"/>
       <c r="P26" s="77">
@@ -4385,7 +4391,7 @@
       </c>
       <c r="Q26" s="75"/>
       <c r="U26" s="67">
-        <f>SUM(R26:T26)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V26" s="31"/>
@@ -4393,16 +4399,16 @@
         <v>0</v>
       </c>
       <c r="X26" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W26,F$2:F$85)</f>
-        <v>366</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W26,F$2:F$86)</f>
+        <v>370</v>
       </c>
       <c r="Y26" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W26,E$2:E$85)</f>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W26,E$2:E$86)</f>
         <v>29</v>
       </c>
       <c r="Z26" s="8">
-        <f t="shared" ref="Z26:Z34" si="0">($Y$17 + $Y$15*X26+$Y$16*Y26)*(1+Y$18+Y$19)</f>
-        <v>39</v>
+        <f t="shared" ref="Z26:Z34" si="2">($Y$17 + $Y$15*X26+$Y$16*Y26)*(1+Y$18+Y$19)</f>
+        <v>39.26</v>
       </c>
       <c r="AA26" s="31"/>
       <c r="AB26" s="31"/>
@@ -4411,10 +4417,10 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B27" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D27" s="13">
         <v>3</v>
@@ -4423,7 +4429,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="13">
-        <f>CEILING(D27,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K27" s="21"/>
@@ -4438,24 +4444,24 @@
         <v>0.2</v>
       </c>
       <c r="U27" s="67">
-        <f>SUM(R27:T27)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.2</v>
       </c>
       <c r="V27" s="31"/>
       <c r="W27" s="69">
         <v>0.5</v>
       </c>
       <c r="X27" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W27,F$2:F$85)</f>
-        <v>228</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W27,F$2:F$86)</f>
+        <v>270</v>
       </c>
       <c r="Y27" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W27,E$2:E$85)</f>
-        <v>22</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W27,E$2:E$86)</f>
+        <v>26</v>
       </c>
       <c r="Z27" s="8">
         <f>($Y$17 + $Y$15*X27+$Y$16*Y27)*(1+Y$18+Y$19)</f>
-        <v>27.3</v>
+        <v>31.590000000000003</v>
       </c>
       <c r="AA27" s="31"/>
       <c r="AB27" s="31"/>
@@ -4468,7 +4474,7 @@
         <v>120</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D28" s="13">
         <v>3</v>
@@ -4477,7 +4483,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="13">
-        <f>CEILING(D28,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G28" s="13"/>
@@ -4515,23 +4521,23 @@
       <c r="S28" s="75"/>
       <c r="T28" s="75"/>
       <c r="U28" s="67">
-        <f>SUM(R28:T28)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="W28" s="69">
         <v>1</v>
       </c>
       <c r="X28" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W28,F$2:F$85)</f>
-        <v>222</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W28,F$2:F$86)</f>
+        <v>244</v>
       </c>
       <c r="Y28" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W28,E$2:E$85)</f>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W28,E$2:E$86)</f>
         <v>22</v>
       </c>
       <c r="Z28" s="8">
-        <f t="shared" si="0"/>
-        <v>26.910000000000004</v>
+        <f t="shared" si="2"/>
+        <v>28.340000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
@@ -4539,7 +4545,7 @@
         <v>121</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D29" s="13">
         <v>3</v>
@@ -4548,7 +4554,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="13">
-        <f>CEILING(D29,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H29" s="13">
@@ -4585,24 +4591,24 @@
         <v>1</v>
       </c>
       <c r="U29" s="67">
-        <f>SUM(R29:T29)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="V29" s="31"/>
       <c r="W29" s="70">
         <v>1.5</v>
       </c>
       <c r="X29" s="29">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W29,F$2:F$85)</f>
-        <v>102</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W29,F$2:F$86)</f>
+        <v>172</v>
       </c>
       <c r="Y29" s="29">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W29,E$2:E$85)</f>
-        <v>13</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W29,E$2:E$86)</f>
+        <v>16</v>
       </c>
       <c r="Z29" s="8">
-        <f t="shared" si="0"/>
-        <v>15.600000000000003</v>
+        <f t="shared" si="2"/>
+        <v>21.32</v>
       </c>
       <c r="AA29" s="31"/>
       <c r="AB29" s="31"/>
@@ -4614,7 +4620,7 @@
         <v>122</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D30" s="13">
         <v>5</v>
@@ -4623,7 +4629,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="13">
-        <f>CEILING(D30,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G30" s="13">
@@ -4641,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="U30" s="67">
-        <f>SUM(R30:T30)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V30" s="31"/>
@@ -4649,16 +4655,16 @@
         <v>2</v>
       </c>
       <c r="X30" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W30,F$2:F$85)</f>
-        <v>98</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W30,F$2:F$86)</f>
+        <v>166</v>
       </c>
       <c r="Y30" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W30,E$2:E$85)</f>
-        <v>13</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W30,E$2:E$86)</f>
+        <v>16</v>
       </c>
       <c r="Z30" s="8">
-        <f t="shared" si="0"/>
-        <v>15.340000000000002</v>
+        <f t="shared" si="2"/>
+        <v>20.930000000000003</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
@@ -4666,7 +4672,7 @@
         <v>123</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D31" s="13">
         <v>5</v>
@@ -4675,7 +4681,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="13">
-        <f>CEILING(D31,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="K31" s="55" t="s">
@@ -4691,7 +4697,7 @@
       </c>
       <c r="T31" s="78"/>
       <c r="U31" s="81">
-        <f>SUM(R31:T31)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V31" s="31"/>
@@ -4699,16 +4705,16 @@
         <v>2.5</v>
       </c>
       <c r="X31" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W31,F$2:F$85)</f>
-        <v>8</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W31,F$2:F$86)</f>
+        <v>66</v>
       </c>
       <c r="Y31" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W31,E$2:E$85)</f>
-        <v>2</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W31,E$2:E$86)</f>
+        <v>6</v>
       </c>
       <c r="Z31" s="8">
-        <f t="shared" si="0"/>
-        <v>5.2</v>
+        <f t="shared" si="2"/>
+        <v>10.530000000000003</v>
       </c>
       <c r="AA31" s="31"/>
       <c r="AB31" s="31"/>
@@ -4723,7 +4729,7 @@
         <v>124</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D32" s="12">
         <v>3</v>
@@ -4732,7 +4738,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="12">
-        <f>CEILING(D32,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G32" s="12">
@@ -4756,7 +4762,7 @@
       <c r="S32" s="76"/>
       <c r="T32" s="77"/>
       <c r="U32" s="67">
-        <f>SUM(R32:T32)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V32" s="31"/>
@@ -4764,16 +4770,16 @@
         <v>3</v>
       </c>
       <c r="X32" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W32,F$2:F$85)</f>
-        <v>8</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W32,F$2:F$86)</f>
+        <v>66</v>
       </c>
       <c r="Y32" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W32,E$2:E$85)</f>
-        <v>2</v>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W32,E$2:E$86)</f>
+        <v>6</v>
       </c>
       <c r="Z32" s="8">
-        <f t="shared" si="0"/>
-        <v>5.2</v>
+        <f t="shared" si="2"/>
+        <v>10.530000000000003</v>
       </c>
     </row>
     <row r="33" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4782,7 +4788,7 @@
         <v>125</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D33" s="13">
         <v>2</v>
@@ -4791,7 +4797,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="13">
-        <f>CEILING(D33,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G33" s="13">
@@ -4835,23 +4841,23 @@
       </c>
       <c r="T33" s="75"/>
       <c r="U33" s="67">
-        <f>SUM(R33:T33)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="V33" s="31"/>
       <c r="W33" s="69">
         <v>3.5</v>
       </c>
       <c r="X33" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W33,F$2:F$85)</f>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W33,F$2:F$86)</f>
         <v>8</v>
       </c>
       <c r="Y33" s="6">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W33,E$2:E$85)</f>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W33,E$2:E$86)</f>
         <v>2</v>
       </c>
       <c r="Z33" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.2</v>
       </c>
       <c r="AA33"/>
@@ -4864,7 +4870,7 @@
         <v>185</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D34" s="13">
         <v>1</v>
@@ -4873,7 +4879,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="13">
-        <f>CEILING(D34,W$22+1)</f>
+        <f t="shared" ref="F34:F66" si="3">CEILING(D34,W$22+1)</f>
         <v>2</v>
       </c>
       <c r="J34" s="13">
@@ -4907,23 +4913,23 @@
         <v>1</v>
       </c>
       <c r="U34" s="67">
-        <f>SUM(R34:T34)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="V34" s="31"/>
       <c r="W34" s="71">
         <v>4</v>
       </c>
       <c r="X34" s="45">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W34,F$2:F$85)</f>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W34,F$2:F$86)</f>
         <v>8</v>
       </c>
       <c r="Y34" s="45">
-        <f>SUMIF(U$2:U$85,"&gt;=" &amp; W34,E$2:E$85)</f>
+        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W34,E$2:E$86)</f>
         <v>2</v>
       </c>
       <c r="Z34" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.2</v>
       </c>
     </row>
@@ -4933,7 +4939,7 @@
         <v>186</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D35" s="13">
         <v>3</v>
@@ -4942,7 +4948,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="13">
-        <f>CEILING(D35,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G35" s="13">
@@ -4986,8 +4992,8 @@
       </c>
       <c r="T35" s="75"/>
       <c r="U35" s="67">
-        <f>SUM(R35:T35)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="W35" s="3"/>
       <c r="X35"/>
@@ -5003,7 +5009,7 @@
         <v>126</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D36" s="13">
         <v>3</v>
@@ -5012,7 +5018,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="13">
-        <f>CEILING(D36,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G36" s="13">
@@ -5035,7 +5041,7 @@
         <v>0</v>
       </c>
       <c r="U36" s="67">
-        <f>SUM(R36:T36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V36" s="31"/>
@@ -5049,7 +5055,7 @@
         <v>97</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D37" s="13">
         <v>2</v>
@@ -5058,7 +5064,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="13">
-        <f>CEILING(D37,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H37" s="13">
@@ -5089,8 +5095,8 @@
         <v>1</v>
       </c>
       <c r="U37" s="67">
-        <f>SUM(R37:T37)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="V37" s="31"/>
       <c r="X37" s="31"/>
@@ -5102,7 +5108,7 @@
         <v>98</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D38" s="13">
         <v>4</v>
@@ -5111,7 +5117,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="13">
-        <f>CEILING(D38,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="J38" s="13">
@@ -5136,8 +5142,8 @@
         <v>1</v>
       </c>
       <c r="U38" s="67">
-        <f>SUM(R38:T38)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="V38" s="31"/>
       <c r="AA38" s="31"/>
@@ -5150,7 +5156,7 @@
         <v>95</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D39" s="13">
         <v>3</v>
@@ -5159,7 +5165,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="13">
-        <f>CEILING(D39,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="J39" s="13">
@@ -5187,8 +5193,8 @@
         <v>1</v>
       </c>
       <c r="U39" s="67">
-        <f>SUM(R39:T39)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="V39" s="31"/>
       <c r="W39" s="72"/>
@@ -5198,7 +5204,7 @@
         <v>127</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D40" s="13">
         <v>7</v>
@@ -5207,7 +5213,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="13">
-        <f>CEILING(D40,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G40" s="13">
@@ -5223,7 +5229,7 @@
         <v>21</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L40" s="32">
         <v>1</v>
@@ -5251,8 +5257,8 @@
       </c>
       <c r="T40" s="78"/>
       <c r="U40" s="81">
-        <f>SUM(R40:T40)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="V40" s="31"/>
       <c r="W40" s="72"/>
@@ -5265,7 +5271,7 @@
         <v>128</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D41" s="12">
         <v>2</v>
@@ -5274,7 +5280,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="12">
-        <f>CEILING(D41,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G41" s="12" t="s">
@@ -5318,8 +5324,8 @@
       </c>
       <c r="T41" s="77"/>
       <c r="U41" s="67">
-        <f>SUM(R41:T41)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="V41" s="31"/>
       <c r="W41" s="72"/>
@@ -5331,7 +5337,7 @@
         <v>170</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D42" s="13">
         <v>5</v>
@@ -5340,7 +5346,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="13">
-        <f>CEILING(D42,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G42" s="13">
@@ -5380,8 +5386,8 @@
       </c>
       <c r="T42" s="75"/>
       <c r="U42" s="67">
-        <f>SUM(R42:T42)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="V42" s="31"/>
       <c r="W42" s="3"/>
@@ -5398,7 +5404,7 @@
         <v>188</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D43" s="13">
         <v>4</v>
@@ -5407,7 +5413,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="13">
-        <f>CEILING(D43,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="K43" s="21" t="s">
@@ -5417,7 +5423,7 @@
       <c r="P43" s="77"/>
       <c r="Q43" s="31"/>
       <c r="U43" s="67">
-        <f>SUM(R43:T43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V43" s="31"/>
@@ -5429,7 +5435,7 @@
         <v>129</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D44" s="13">
         <v>6</v>
@@ -5438,7 +5444,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="13">
-        <f>CEILING(D44,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H44" s="13">
@@ -5470,18 +5476,18 @@
         <v>1</v>
       </c>
       <c r="U44" s="67">
-        <f>SUM(R44:T44)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="V44" s="31"/>
       <c r="Z44" s="6"/>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B45" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D45" s="13">
         <v>5</v>
@@ -5490,7 +5496,7 @@
         <v>2</v>
       </c>
       <c r="F45" s="13">
-        <f>CEILING(D45,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G45" s="13" t="s">
@@ -5528,8 +5534,8 @@
       </c>
       <c r="T45" s="78"/>
       <c r="U45" s="81">
-        <f>SUM(R45:T45)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="V45" s="31"/>
     </row>
@@ -5538,10 +5544,10 @@
         <v>79</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D46" s="12">
         <v>7</v>
@@ -5550,7 +5556,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="12">
-        <f>CEILING(D46,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G46" s="12" t="s">
@@ -5566,7 +5572,7 @@
         <v>26</v>
       </c>
       <c r="K46" s="20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="L46" s="33">
         <v>1</v>
@@ -5590,18 +5596,18 @@
       <c r="S46" s="76"/>
       <c r="T46" s="77"/>
       <c r="U46" s="67">
-        <f>SUM(R46:T46)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.8</v>
       </c>
       <c r="W46" s="3"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A47" s="28"/>
       <c r="B47" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D47" s="13">
         <v>4</v>
@@ -5610,11 +5616,11 @@
         <v>2</v>
       </c>
       <c r="F47" s="13">
-        <f>CEILING(D47,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L47" s="77"/>
       <c r="M47" s="77"/>
@@ -5630,7 +5636,7 @@
       </c>
       <c r="T47" s="77"/>
       <c r="U47" s="67">
-        <f>SUM(R47:T47)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V47" s="31"/>
@@ -5646,7 +5652,7 @@
         <v>93</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D48" s="13">
         <v>6</v>
@@ -5655,7 +5661,7 @@
         <v>3</v>
       </c>
       <c r="F48" s="13">
-        <f>CEILING(D48,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G48" s="13" t="s">
@@ -5671,7 +5677,7 @@
         <v>27</v>
       </c>
       <c r="K48" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="L48" s="32">
         <v>1</v>
@@ -5695,8 +5701,8 @@
       <c r="S48" s="75"/>
       <c r="T48" s="75"/>
       <c r="U48" s="67">
-        <f>SUM(R48:T48)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.8</v>
       </c>
       <c r="W48" s="3"/>
       <c r="Z48" s="6"/>
@@ -5708,10 +5714,10 @@
     <row r="49" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="10"/>
       <c r="B49" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C49" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D49" s="13">
         <v>8</v>
@@ -5720,7 +5726,7 @@
         <v>4</v>
       </c>
       <c r="F49" s="13">
-        <f>CEILING(D49,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G49" s="13"/>
@@ -5728,7 +5734,7 @@
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
       <c r="K49" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L49" s="75"/>
       <c r="M49" s="75"/>
@@ -5744,7 +5750,7 @@
       </c>
       <c r="T49" s="75"/>
       <c r="U49" s="67">
-        <f>SUM(R49:T49)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V49" s="31"/>
@@ -5761,7 +5767,7 @@
         <v>130</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D50" s="13">
         <v>2</v>
@@ -5770,7 +5776,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="13">
-        <f>CEILING(D50,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G50" s="13">
@@ -5808,18 +5814,18 @@
         <v>1</v>
       </c>
       <c r="U50" s="67">
-        <f>SUM(R50:T50)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>1.8</v>
       </c>
       <c r="V50" s="31"/>
       <c r="Y50" s="6"/>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B51" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D51" s="13">
         <v>4</v>
@@ -5828,7 +5834,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="13">
-        <f>CEILING(D51,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G51" s="13">
@@ -5844,7 +5850,7 @@
         <v>28</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L51" s="32"/>
       <c r="N51" s="75">
@@ -5859,7 +5865,7 @@
       <c r="Q51" s="32"/>
       <c r="T51" s="78"/>
       <c r="U51" s="81">
-        <f>SUM(R51:T51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V51" s="31"/>
@@ -5869,10 +5875,10 @@
         <v>80</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D52" s="12">
         <v>2</v>
@@ -5881,7 +5887,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="12">
-        <f>CEILING(D52,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G52" s="12">
@@ -5913,7 +5919,7 @@
       </c>
       <c r="T52" s="77"/>
       <c r="U52" s="67">
-        <f>SUM(R52:T52)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V52" s="31"/>
@@ -5931,7 +5937,7 @@
         <v>131</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D53" s="13">
         <v>3</v>
@@ -5940,7 +5946,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="13">
-        <f>CEILING(D53,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G53" s="13">
@@ -5970,7 +5976,7 @@
       </c>
       <c r="T53" s="78"/>
       <c r="U53" s="81">
-        <f>SUM(R53:T53)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V53" s="31"/>
@@ -5983,7 +5989,7 @@
         <v>132</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D54" s="12">
         <v>2</v>
@@ -5992,7 +5998,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="12">
-        <f>CEILING(D54,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G54" s="12"/>
@@ -6026,7 +6032,7 @@
       </c>
       <c r="T54" s="77"/>
       <c r="U54" s="67">
-        <f>SUM(R54:T54)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V54" s="31"/>
@@ -6042,7 +6048,7 @@
         <v>133</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D55" s="13">
         <v>3</v>
@@ -6051,7 +6057,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="13">
-        <f>CEILING(D55,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G55" s="13">
@@ -6089,7 +6095,7 @@
         <v>1</v>
       </c>
       <c r="U55" s="67">
-        <f>SUM(R55:T55)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V55" s="31"/>
@@ -6099,7 +6105,7 @@
         <v>134</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D56" s="13">
         <v>3</v>
@@ -6108,7 +6114,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="13">
-        <f>CEILING(D56,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G56" s="13">
@@ -6137,7 +6143,7 @@
         <v>1</v>
       </c>
       <c r="U56" s="67">
-        <f>SUM(R56:T56)</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="V56" s="31"/>
@@ -6151,7 +6157,7 @@
         <v>135</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D57" s="13">
         <v>3</v>
@@ -6160,7 +6166,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="13">
-        <f>CEILING(D57,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G57" s="13">
@@ -6178,7 +6184,7 @@
         <v>1</v>
       </c>
       <c r="U57" s="67">
-        <f>SUM(R57:T57)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V57" s="31"/>
@@ -6189,7 +6195,7 @@
         <v>136</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D58" s="13">
         <v>2</v>
@@ -6198,7 +6204,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="13">
-        <f>CEILING(D58,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G58" s="13">
@@ -6236,8 +6242,8 @@
         <v>1</v>
       </c>
       <c r="U58" s="67">
-        <f>SUM(R58:T58)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>2.2000000000000002</v>
       </c>
       <c r="V58" s="31"/>
       <c r="AA58" s="31"/>
@@ -6247,7 +6253,7 @@
         <v>137</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D59" s="13">
         <v>5</v>
@@ -6256,7 +6262,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="13">
-        <f>CEILING(D59,W$22+1)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G59" s="13">
@@ -6285,7 +6291,7 @@
         <v>1</v>
       </c>
       <c r="P59" s="77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q59" s="73">
         <v>1</v>
@@ -6294,228 +6300,231 @@
         <v>1</v>
       </c>
       <c r="U59" s="67">
-        <f>SUM(R59:T59)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="V59" s="31"/>
       <c r="Y59" s="6"/>
       <c r="AA59" s="31"/>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B60" s="22" t="s">
+    <row r="60" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="10"/>
+      <c r="B60" t="s">
+        <v>237</v>
+      </c>
+      <c r="C60" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" s="13">
+        <v>4</v>
+      </c>
+      <c r="E60" s="13">
+        <v>0</v>
+      </c>
+      <c r="F60" s="13">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="L60" s="75"/>
+      <c r="M60" s="75"/>
+      <c r="N60" s="75"/>
+      <c r="O60" s="75"/>
+      <c r="P60" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="73"/>
+      <c r="R60" s="75"/>
+      <c r="S60" s="75"/>
+      <c r="T60" s="75"/>
+      <c r="U60" s="67">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W60" s="3"/>
+      <c r="Y60" s="6"/>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B61" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="C60" s="29" t="s">
-        <v>204</v>
-      </c>
-      <c r="D60" s="13">
+      <c r="C61" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D61" s="13">
         <v>5</v>
       </c>
-      <c r="E60" s="13">
-        <v>0</v>
-      </c>
-      <c r="F60" s="13">
-        <f>CEILING(D60,W$22+1)</f>
+      <c r="E61" s="13">
+        <v>0</v>
+      </c>
+      <c r="F61" s="13">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="G60" s="13">
+      <c r="G61" s="13">
         <v>9</v>
       </c>
-      <c r="H60" s="13">
+      <c r="H61" s="13">
         <v>36</v>
       </c>
-      <c r="I60" s="13">
+      <c r="I61" s="13">
         <v>5</v>
       </c>
-      <c r="J60" s="13">
+      <c r="J61" s="13">
         <v>34</v>
       </c>
-      <c r="K60" s="21"/>
-      <c r="L60" s="32">
-        <v>1</v>
-      </c>
-      <c r="M60" s="75">
-        <v>1</v>
-      </c>
-      <c r="N60" s="75">
+      <c r="K61" s="21"/>
+      <c r="L61" s="32">
+        <v>1</v>
+      </c>
+      <c r="M61" s="75">
+        <v>1</v>
+      </c>
+      <c r="N61" s="75">
         <v>0.5</v>
       </c>
-      <c r="P60" s="77">
+      <c r="P61" s="77">
         <v>0.1</v>
       </c>
-      <c r="Q60" s="73">
-        <v>1</v>
-      </c>
-      <c r="R60" s="75">
-        <v>1</v>
-      </c>
-      <c r="U60" s="67">
-        <f>SUM(R60:T60)</f>
-        <v>1</v>
-      </c>
-      <c r="V60" s="31"/>
-      <c r="AA60" s="31"/>
-    </row>
-    <row r="61" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="10"/>
-      <c r="B61" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="C61" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="D61" s="13">
+      <c r="Q61" s="73">
+        <v>1</v>
+      </c>
+      <c r="R61" s="75">
+        <v>1</v>
+      </c>
+      <c r="U61" s="67">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="V61" s="31"/>
+      <c r="AA61" s="31"/>
+    </row>
+    <row r="62" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="10"/>
+      <c r="B62" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C62" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="D62" s="13">
         <v>3</v>
       </c>
-      <c r="E61" s="13">
-        <v>0</v>
-      </c>
-      <c r="F61" s="13">
-        <f>CEILING(D61,W$22+1)</f>
+      <c r="E62" s="13">
+        <v>0</v>
+      </c>
+      <c r="F62" s="13">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
-      <c r="K61" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="L61" s="75"/>
-      <c r="M61" s="75"/>
-      <c r="N61" s="75"/>
-      <c r="O61" s="75"/>
-      <c r="P61" s="77"/>
-      <c r="Q61" s="73"/>
-      <c r="R61" s="75"/>
-      <c r="S61" s="75"/>
-      <c r="T61" s="75"/>
-      <c r="U61" s="67">
-        <f>SUM(R61:T61)</f>
-        <v>0</v>
-      </c>
-      <c r="W61" s="3"/>
-    </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B62" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="C62" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="D62" s="13">
-        <v>1</v>
-      </c>
-      <c r="E62" s="13">
-        <v>0</v>
-      </c>
-      <c r="F62" s="13">
-        <f>CEILING(D62,W$22+1)</f>
-        <v>2</v>
-      </c>
-      <c r="H62" s="13">
-        <v>37</v>
-      </c>
-      <c r="J62" s="13">
-        <v>35</v>
-      </c>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
       <c r="K62" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="L62" s="32">
-        <v>1</v>
-      </c>
-      <c r="M62" s="75">
-        <v>1</v>
-      </c>
-      <c r="N62" s="75">
-        <v>1</v>
-      </c>
-      <c r="O62" s="75">
-        <v>1</v>
-      </c>
-      <c r="P62" s="77">
-        <v>1</v>
-      </c>
-      <c r="Q62" s="73">
-        <v>1</v>
-      </c>
-      <c r="R62" s="75">
-        <v>1</v>
-      </c>
-      <c r="S62" s="75">
-        <v>1</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="L62" s="75"/>
+      <c r="M62" s="75"/>
+      <c r="N62" s="75"/>
+      <c r="O62" s="75"/>
+      <c r="P62" s="77"/>
+      <c r="Q62" s="73"/>
+      <c r="R62" s="75"/>
+      <c r="S62" s="75"/>
+      <c r="T62" s="75"/>
       <c r="U62" s="67">
-        <f>SUM(R62:T62)</f>
-        <v>2</v>
-      </c>
-      <c r="V62" s="31"/>
-      <c r="Z62" s="6"/>
-      <c r="AA62" s="31"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W62" s="3"/>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B63" s="22" t="s">
-        <v>96</v>
+        <v>235</v>
       </c>
       <c r="C63" s="29" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D63" s="13">
+        <v>1</v>
+      </c>
+      <c r="E63" s="13">
+        <v>0</v>
+      </c>
+      <c r="F63" s="13">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H63" s="13">
+        <v>37</v>
+      </c>
+      <c r="J63" s="13">
+        <v>35</v>
+      </c>
+      <c r="K63" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="L63" s="32">
+        <v>1</v>
+      </c>
+      <c r="M63" s="75">
+        <v>1</v>
+      </c>
+      <c r="N63" s="75">
+        <v>1</v>
+      </c>
+      <c r="O63" s="75">
+        <v>1</v>
+      </c>
+      <c r="P63" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="73">
+        <v>1</v>
+      </c>
+      <c r="R63" s="75">
+        <v>1</v>
+      </c>
+      <c r="S63" s="75">
+        <v>1</v>
+      </c>
+      <c r="U63" s="67">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E63" s="13">
-        <v>0</v>
-      </c>
-      <c r="F63" s="13">
-        <f>CEILING(D63,W$22+1)</f>
-        <v>4</v>
-      </c>
-      <c r="J63" s="13">
-        <v>36</v>
-      </c>
-      <c r="K63" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="L63" s="32">
-        <v>1</v>
-      </c>
-      <c r="N63" s="75">
-        <v>0.5</v>
-      </c>
-      <c r="P63" s="77">
-        <v>0.5</v>
-      </c>
-      <c r="Q63" s="31"/>
-      <c r="U63" s="67">
-        <f>SUM(R63:T63)</f>
-        <v>0</v>
-      </c>
       <c r="V63" s="31"/>
+      <c r="Z63" s="6"/>
       <c r="AA63" s="31"/>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B64" s="22" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="C64" s="29" t="s">
         <v>203</v>
       </c>
       <c r="D64" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E64" s="13">
         <v>0</v>
       </c>
       <c r="F64" s="13">
-        <f>CEILING(D64,W$22+1)</f>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="J64" s="13">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K64" s="21" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
       <c r="L64" s="32">
         <v>1</v>
@@ -6523,17 +6532,12 @@
       <c r="N64" s="75">
         <v>0.5</v>
       </c>
-      <c r="O64" s="75">
-        <v>1</v>
-      </c>
       <c r="P64" s="77">
-        <v>1</v>
-      </c>
-      <c r="Q64" s="32">
         <v>0.5</v>
       </c>
+      <c r="Q64" s="31"/>
       <c r="U64" s="67">
-        <f>SUM(R64:T64)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V64" s="31"/>
@@ -6541,230 +6545,242 @@
     </row>
     <row r="65" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B65" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D65" s="13">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E65" s="13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F65" s="13">
-        <f>CEILING(D65,W$22+1)</f>
-        <v>10</v>
-      </c>
-      <c r="G65" s="13">
-        <v>10</v>
-      </c>
-      <c r="K65" s="21"/>
-      <c r="L65" s="32"/>
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="J65" s="13">
+        <v>37</v>
+      </c>
+      <c r="K65" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L65" s="32">
+        <v>1</v>
+      </c>
+      <c r="N65" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="O65" s="75">
+        <v>1</v>
+      </c>
       <c r="P65" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q65" s="31"/>
-      <c r="R65" s="75">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="Q65" s="32">
+        <v>0.5</v>
       </c>
       <c r="U65" s="67">
-        <f>SUM(R65:T65)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="V65" s="31"/>
       <c r="AA65" s="31"/>
-      <c r="AB65" s="6"/>
-      <c r="AC65" s="6"/>
-      <c r="AD65" s="6"/>
     </row>
     <row r="66" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B66" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D66" s="13">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E66" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F66" s="13">
-        <f>CEILING(D66,W$22+1)</f>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="G66" s="13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K66" s="21"/>
       <c r="L66" s="32"/>
-      <c r="N66" s="75">
-        <v>0</v>
-      </c>
-      <c r="P66" s="77"/>
+      <c r="P66" s="77">
+        <v>0</v>
+      </c>
       <c r="Q66" s="31"/>
       <c r="R66" s="75">
         <v>1</v>
       </c>
       <c r="U66" s="67">
-        <f>SUM(R66:T66)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V66" s="31"/>
-      <c r="Z66" s="6"/>
       <c r="AA66" s="31"/>
+      <c r="AB66" s="6"/>
+      <c r="AC66" s="6"/>
+      <c r="AD66" s="6"/>
     </row>
     <row r="67" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B67" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C67" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D67" s="13">
+        <v>7</v>
+      </c>
+      <c r="E67" s="13">
+        <v>1</v>
+      </c>
+      <c r="F67" s="13">
+        <f t="shared" ref="F67:F85" si="4">CEILING(D67,W$22+1)</f>
+        <v>8</v>
+      </c>
+      <c r="G67" s="13">
+        <v>11</v>
+      </c>
+      <c r="K67" s="21"/>
+      <c r="L67" s="32"/>
+      <c r="N67" s="75">
+        <v>0</v>
+      </c>
+      <c r="P67" s="77"/>
+      <c r="Q67" s="31"/>
+      <c r="R67" s="75">
+        <v>1</v>
+      </c>
+      <c r="U67" s="67">
+        <f t="shared" ref="U67:U85" si="5">SUM(Q67:T67)</f>
+        <v>1</v>
+      </c>
+      <c r="V67" s="31"/>
+      <c r="Z67" s="6"/>
+      <c r="AA67" s="31"/>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B68" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="C67" s="29" t="s">
-        <v>203</v>
-      </c>
-      <c r="D67" s="13">
+      <c r="C68" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D68" s="13">
         <v>5</v>
       </c>
-      <c r="E67" s="13">
-        <v>0</v>
-      </c>
-      <c r="F67" s="13">
-        <f>CEILING(D67,W$22+1)</f>
+      <c r="E68" s="13">
+        <v>0</v>
+      </c>
+      <c r="F68" s="13">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="J67" s="13">
+      <c r="J68" s="13">
         <v>38</v>
       </c>
-      <c r="K67" s="21" t="s">
+      <c r="K68" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="L67" s="32">
-        <v>1</v>
-      </c>
-      <c r="N67" s="75">
+      <c r="L68" s="32">
+        <v>1</v>
+      </c>
+      <c r="N68" s="75">
         <v>0.5</v>
       </c>
-      <c r="O67" s="75">
-        <v>1</v>
-      </c>
-      <c r="P67" s="77">
-        <v>1</v>
-      </c>
-      <c r="Q67" s="32"/>
-      <c r="T67" s="78"/>
-      <c r="U67" s="81">
-        <f>SUM(R67:T67)</f>
-        <v>0</v>
-      </c>
-      <c r="V67" s="31"/>
-      <c r="AA67" s="31"/>
-    </row>
-    <row r="68" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="11" t="s">
+      <c r="O68" s="75">
+        <v>1</v>
+      </c>
+      <c r="P68" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="32"/>
+      <c r="T68" s="78"/>
+      <c r="U68" s="81">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V68" s="31"/>
+      <c r="AA68" s="31"/>
+    </row>
+    <row r="69" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B68" s="25" t="s">
+      <c r="B69" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="C68" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="D68" s="12">
+      <c r="C69" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="D69" s="12">
         <v>3</v>
       </c>
-      <c r="E68" s="12">
-        <v>0</v>
-      </c>
-      <c r="F68" s="12">
-        <f>CEILING(D68,W$22+1)</f>
+      <c r="E69" s="12">
+        <v>0</v>
+      </c>
+      <c r="F69" s="12">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="G68" s="12">
+      <c r="G69" s="12">
         <v>45</v>
       </c>
-      <c r="H68" s="12">
+      <c r="H69" s="12">
         <v>27</v>
       </c>
-      <c r="I68" s="12">
+      <c r="I69" s="12">
         <v>36</v>
       </c>
-      <c r="J68" s="12">
+      <c r="J69" s="12">
         <v>29</v>
       </c>
-      <c r="K68" s="20"/>
-      <c r="L68" s="33"/>
-      <c r="M68" s="76"/>
-      <c r="N68" s="76">
+      <c r="K69" s="20"/>
+      <c r="L69" s="33"/>
+      <c r="M69" s="76"/>
+      <c r="N69" s="76">
         <v>0.5</v>
       </c>
-      <c r="O68" s="76">
-        <v>1</v>
-      </c>
-      <c r="P68" s="76">
+      <c r="O69" s="76">
+        <v>1</v>
+      </c>
+      <c r="P69" s="76">
         <v>0.5</v>
       </c>
-      <c r="Q68" s="33"/>
-      <c r="R68" s="76">
-        <v>1</v>
-      </c>
-      <c r="S68" s="76">
-        <v>1</v>
-      </c>
-      <c r="T68" s="77"/>
-      <c r="U68" s="67">
-        <f>SUM(R68:T68)</f>
+      <c r="Q69" s="33"/>
+      <c r="R69" s="76">
+        <v>1</v>
+      </c>
+      <c r="S69" s="76">
+        <v>1</v>
+      </c>
+      <c r="T69" s="77"/>
+      <c r="U69" s="67">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="V68" s="31"/>
-      <c r="W68" s="3"/>
-      <c r="X68"/>
-      <c r="Y68"/>
-      <c r="Z68"/>
-      <c r="AA68" s="31"/>
-      <c r="AB68"/>
-      <c r="AC68"/>
-      <c r="AD68"/>
-    </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B69" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="C69" s="29" t="s">
-        <v>204</v>
-      </c>
-      <c r="D69" s="13">
-        <v>7</v>
-      </c>
-      <c r="E69" s="13">
-        <v>2</v>
-      </c>
-      <c r="F69" s="13">
-        <f>CEILING(D69,W$22+1)</f>
-        <v>8</v>
-      </c>
-      <c r="G69" s="13">
-        <v>46</v>
-      </c>
-      <c r="K69" s="21"/>
-      <c r="L69" s="32"/>
-      <c r="P69" s="77"/>
-      <c r="Q69" s="31"/>
-      <c r="R69" s="75">
-        <v>1</v>
-      </c>
-      <c r="U69" s="67">
-        <f>SUM(R69:T69)</f>
-        <v>1</v>
-      </c>
       <c r="V69" s="31"/>
+      <c r="W69" s="3"/>
+      <c r="X69"/>
+      <c r="Y69"/>
+      <c r="Z69"/>
+      <c r="AA69" s="31"/>
+      <c r="AB69"/>
+      <c r="AC69"/>
+      <c r="AD69"/>
     </row>
     <row r="70" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B70" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C70" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D70" s="13">
         <v>7</v>
@@ -6773,427 +6789,400 @@
         <v>2</v>
       </c>
       <c r="F70" s="13">
-        <f>CEILING(D70,W$22+1)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G70" s="13">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K70" s="21"/>
       <c r="L70" s="32"/>
       <c r="P70" s="77"/>
       <c r="Q70" s="31"/>
+      <c r="R70" s="75">
+        <v>1</v>
+      </c>
       <c r="U70" s="67">
-        <f>SUM(R70:T70)</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="V70" s="31"/>
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A71" s="46"/>
-      <c r="B71" s="23" t="s">
+      <c r="B71" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="C71" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D71" s="13">
+        <v>7</v>
+      </c>
+      <c r="E71" s="13">
+        <v>2</v>
+      </c>
+      <c r="F71" s="13">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G71" s="13">
+        <v>47</v>
+      </c>
+      <c r="K71" s="21"/>
+      <c r="L71" s="32"/>
+      <c r="P71" s="77"/>
+      <c r="Q71" s="31"/>
+      <c r="U71" s="67">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V71" s="31"/>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A72" s="46"/>
+      <c r="B72" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="C71" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="D71" s="26">
+      <c r="C72" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="D72" s="26">
         <v>10</v>
       </c>
-      <c r="E71" s="26">
-        <v>0</v>
-      </c>
-      <c r="F71" s="26">
-        <f>CEILING(D71,W$22+1)</f>
+      <c r="E72" s="26">
+        <v>0</v>
+      </c>
+      <c r="F72" s="26">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="G71" s="26">
+      <c r="G72" s="26">
         <v>34</v>
       </c>
-      <c r="H71" s="26"/>
-      <c r="I71" s="26"/>
-      <c r="J71" s="26"/>
-      <c r="K71" s="27"/>
-      <c r="L71" s="35"/>
-      <c r="M71" s="78"/>
-      <c r="N71" s="78"/>
-      <c r="O71" s="78">
-        <v>1</v>
-      </c>
-      <c r="P71" s="78"/>
-      <c r="Q71" s="35"/>
-      <c r="R71" s="78">
-        <v>1</v>
-      </c>
-      <c r="S71" s="78"/>
-      <c r="T71" s="78"/>
-      <c r="U71" s="81">
-        <f>SUM(R71:T71)</f>
-        <v>1</v>
-      </c>
-      <c r="V71" s="31"/>
-      <c r="X71" s="31"/>
-      <c r="Z71" s="6"/>
-    </row>
-    <row r="72" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="10" t="s">
+      <c r="H72" s="26"/>
+      <c r="I72" s="26"/>
+      <c r="J72" s="26"/>
+      <c r="K72" s="27"/>
+      <c r="L72" s="35"/>
+      <c r="M72" s="78"/>
+      <c r="N72" s="78"/>
+      <c r="O72" s="78">
+        <v>1</v>
+      </c>
+      <c r="P72" s="78"/>
+      <c r="Q72" s="35"/>
+      <c r="R72" s="78">
+        <v>1</v>
+      </c>
+      <c r="S72" s="78"/>
+      <c r="T72" s="78"/>
+      <c r="U72" s="81">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="V72" s="31"/>
+      <c r="X72" s="31"/>
+      <c r="Z72" s="6"/>
+    </row>
+    <row r="73" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B72" s="22" t="s">
+      <c r="B73" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="C72" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="D72" s="13">
+      <c r="C73" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="D73" s="13">
         <v>4</v>
       </c>
-      <c r="E72" s="13">
-        <v>0</v>
-      </c>
-      <c r="F72" s="13">
-        <f>CEILING(D72,W$22+1)</f>
+      <c r="E73" s="13">
+        <v>0</v>
+      </c>
+      <c r="F73" s="13">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="G72" s="13">
+      <c r="G73" s="13">
         <v>48</v>
       </c>
-      <c r="H72" s="13"/>
-      <c r="I72" s="13"/>
-      <c r="J72" s="13"/>
-      <c r="K72" s="21"/>
-      <c r="L72" s="32"/>
-      <c r="M72" s="75"/>
-      <c r="N72" s="75"/>
-      <c r="O72" s="75"/>
-      <c r="P72" s="77"/>
-      <c r="Q72" s="31"/>
-      <c r="R72" s="75"/>
-      <c r="S72" s="75"/>
-      <c r="T72" s="75"/>
-      <c r="U72" s="67">
-        <f>SUM(R72:T72)</f>
-        <v>0</v>
-      </c>
-      <c r="V72" s="31"/>
-      <c r="W72" s="3"/>
-      <c r="X72"/>
-      <c r="Y72"/>
-      <c r="Z72"/>
-      <c r="AA72"/>
-      <c r="AB72"/>
-      <c r="AC72"/>
-      <c r="AD72"/>
-    </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B73" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="C73" s="29" t="s">
-        <v>203</v>
-      </c>
-      <c r="D73" s="13">
-        <v>3</v>
-      </c>
-      <c r="E73" s="13">
-        <v>0</v>
-      </c>
-      <c r="F73" s="13">
-        <f>CEILING(D73,W$22+1)</f>
-        <v>4</v>
-      </c>
-      <c r="G73" s="13">
-        <v>49</v>
-      </c>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
       <c r="K73" s="21"/>
       <c r="L73" s="32"/>
+      <c r="M73" s="75"/>
+      <c r="N73" s="75"/>
+      <c r="O73" s="75"/>
       <c r="P73" s="77"/>
-      <c r="Q73" s="32"/>
+      <c r="Q73" s="31"/>
+      <c r="R73" s="75"/>
+      <c r="S73" s="75"/>
+      <c r="T73" s="75"/>
       <c r="U73" s="67">
-        <f>SUM(R73:T73)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V73" s="31"/>
-      <c r="AA73" s="6"/>
-      <c r="AB73" s="6"/>
-      <c r="AC73" s="6"/>
-      <c r="AD73" s="6"/>
-    </row>
-    <row r="74" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="10"/>
+      <c r="W73" s="3"/>
+      <c r="X73"/>
+      <c r="Y73"/>
+      <c r="Z73"/>
+      <c r="AA73"/>
+      <c r="AB73"/>
+      <c r="AC73"/>
+      <c r="AD73"/>
+    </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B74" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D74" s="13">
+        <v>3</v>
+      </c>
+      <c r="E74" s="13">
+        <v>0</v>
+      </c>
+      <c r="F74" s="13">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G74" s="13">
+        <v>49</v>
+      </c>
+      <c r="K74" s="21"/>
+      <c r="L74" s="32"/>
+      <c r="P74" s="77"/>
+      <c r="Q74" s="32"/>
+      <c r="U74" s="67">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V74" s="31"/>
+      <c r="AA74" s="6"/>
+      <c r="AB74" s="6"/>
+      <c r="AC74" s="6"/>
+      <c r="AD74" s="6"/>
+    </row>
+    <row r="75" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="10"/>
+      <c r="B75" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="D75" s="13">
+        <v>4</v>
+      </c>
+      <c r="E75" s="13">
+        <v>0</v>
+      </c>
+      <c r="F75" s="13">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="C74" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="D74" s="13">
-        <v>4</v>
-      </c>
-      <c r="E74" s="13">
-        <v>0</v>
-      </c>
-      <c r="F74" s="13">
-        <f>CEILING(D74,W$22+1)</f>
-        <v>4</v>
-      </c>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="L74" s="75"/>
-      <c r="M74" s="75"/>
-      <c r="N74" s="75"/>
-      <c r="O74" s="75"/>
-      <c r="P74" s="77"/>
-      <c r="Q74" s="75"/>
-      <c r="R74" s="75"/>
-      <c r="S74" s="75"/>
-      <c r="T74" s="78"/>
-      <c r="U74" s="81">
-        <f>SUM(R74:T74)</f>
-        <v>0</v>
-      </c>
-      <c r="W74" s="3"/>
-      <c r="X74"/>
-      <c r="Y74"/>
-      <c r="Z74"/>
-      <c r="AA74"/>
-      <c r="AB74"/>
-      <c r="AC74"/>
-      <c r="AD74"/>
-    </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A75" s="11" t="s">
+      <c r="L75" s="75"/>
+      <c r="M75" s="75"/>
+      <c r="N75" s="75"/>
+      <c r="O75" s="75"/>
+      <c r="P75" s="77"/>
+      <c r="Q75" s="75"/>
+      <c r="R75" s="75"/>
+      <c r="S75" s="75"/>
+      <c r="T75" s="78"/>
+      <c r="U75" s="81">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W75" s="3"/>
+      <c r="X75"/>
+      <c r="Y75"/>
+      <c r="Z75"/>
+      <c r="AA75"/>
+      <c r="AB75"/>
+      <c r="AC75"/>
+      <c r="AD75"/>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A76" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B75" s="25" t="s">
+      <c r="B76" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C75" s="25"/>
-      <c r="D75" s="12">
+      <c r="C76" s="25"/>
+      <c r="D76" s="12">
         <v>2</v>
       </c>
-      <c r="E75" s="12">
-        <v>0</v>
-      </c>
-      <c r="F75" s="12">
-        <f>CEILING(D75,W$22+1)</f>
+      <c r="E76" s="12">
+        <v>0</v>
+      </c>
+      <c r="F76" s="12">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="12"/>
-      <c r="K75" s="20"/>
-      <c r="L75" s="33">
-        <v>1</v>
-      </c>
-      <c r="M75" s="76">
-        <v>1</v>
-      </c>
-      <c r="N75" s="76">
-        <v>1</v>
-      </c>
-      <c r="O75" s="76">
-        <v>1</v>
-      </c>
-      <c r="P75" s="76">
-        <v>0</v>
-      </c>
-      <c r="Q75" s="33">
-        <v>1</v>
-      </c>
-      <c r="R75" s="76"/>
-      <c r="S75" s="76"/>
-      <c r="T75" s="77"/>
-      <c r="U75" s="67">
-        <f>SUM(R75:T75)</f>
-        <v>0</v>
-      </c>
-      <c r="V75" s="31"/>
-    </row>
-    <row r="76" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="28"/>
-      <c r="B76" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="C76" s="29"/>
-      <c r="D76" s="13">
-        <v>2</v>
-      </c>
-      <c r="E76" s="13">
-        <v>1</v>
-      </c>
-      <c r="F76" s="13">
-        <f>CEILING(D76,W$22+1)</f>
-        <v>2</v>
-      </c>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="13"/>
-      <c r="K76" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="L76" s="34"/>
-      <c r="M76" s="77">
-        <v>1</v>
-      </c>
-      <c r="N76" s="77">
-        <v>1</v>
-      </c>
-      <c r="O76" s="77">
-        <v>1</v>
-      </c>
-      <c r="P76" s="77">
-        <v>1</v>
-      </c>
-      <c r="Q76" s="34">
-        <v>1</v>
-      </c>
-      <c r="R76" s="77">
-        <v>1</v>
-      </c>
-      <c r="S76" s="77">
-        <v>1</v>
-      </c>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="20"/>
+      <c r="L76" s="33">
+        <v>1</v>
+      </c>
+      <c r="M76" s="76">
+        <v>1</v>
+      </c>
+      <c r="N76" s="76">
+        <v>1</v>
+      </c>
+      <c r="O76" s="76">
+        <v>1</v>
+      </c>
+      <c r="P76" s="76">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="33">
+        <v>1</v>
+      </c>
+      <c r="R76" s="76"/>
+      <c r="S76" s="76"/>
       <c r="T76" s="77"/>
       <c r="U76" s="67">
-        <f>SUM(R76:T76)</f>
-        <v>2</v>
-      </c>
-      <c r="W76" s="3"/>
-    </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="V76" s="31"/>
+    </row>
+    <row r="77" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="28"/>
       <c r="B77" s="29" t="s">
-        <v>212</v>
+        <v>99</v>
       </c>
       <c r="C77" s="29"/>
       <c r="D77" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E77" s="13">
         <v>1</v>
       </c>
       <c r="F77" s="13">
-        <f>CEILING(D77,W$22+1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
       <c r="K77" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="L77" s="77"/>
-      <c r="M77" s="77"/>
-      <c r="N77" s="77"/>
-      <c r="O77" s="77"/>
+        <v>204</v>
+      </c>
+      <c r="L77" s="34"/>
+      <c r="M77" s="77">
+        <v>1</v>
+      </c>
+      <c r="N77" s="77">
+        <v>1</v>
+      </c>
+      <c r="O77" s="77">
+        <v>1</v>
+      </c>
       <c r="P77" s="77">
         <v>1</v>
       </c>
-      <c r="Q77" s="77"/>
+      <c r="Q77" s="34">
+        <v>1</v>
+      </c>
       <c r="R77" s="77">
         <v>1</v>
       </c>
       <c r="S77" s="77">
         <v>1</v>
       </c>
-      <c r="T77" s="77">
+      <c r="T77" s="77"/>
+      <c r="U77" s="67">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="W77" s="3"/>
+    </row>
+    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A78" s="28"/>
+      <c r="B78" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C78" s="29"/>
+      <c r="D78" s="13">
+        <v>1</v>
+      </c>
+      <c r="E78" s="13">
+        <v>1</v>
+      </c>
+      <c r="F78" s="13">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="U77" s="67">
-        <f>SUM(R77:T77)</f>
+      <c r="K78" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="L78" s="77"/>
+      <c r="M78" s="77"/>
+      <c r="N78" s="77"/>
+      <c r="O78" s="77"/>
+      <c r="P78" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q78" s="77"/>
+      <c r="R78" s="77">
+        <v>1</v>
+      </c>
+      <c r="S78" s="77">
+        <v>1</v>
+      </c>
+      <c r="T78" s="77">
+        <v>2</v>
+      </c>
+      <c r="U78" s="67">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="V77" s="31"/>
-      <c r="X77" s="31"/>
-      <c r="Y77" s="31"/>
-      <c r="Z77" s="31"/>
-    </row>
-    <row r="78" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="10"/>
-      <c r="B78" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="C78" s="22"/>
-      <c r="D78" s="13">
-        <v>4</v>
-      </c>
-      <c r="E78" s="13">
-        <v>3</v>
-      </c>
-      <c r="F78" s="13">
-        <f>CEILING(D78,W$22+1)</f>
-        <v>4</v>
-      </c>
-      <c r="G78" s="13"/>
-      <c r="H78" s="13"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="13"/>
-      <c r="K78" s="21"/>
-      <c r="L78" s="32">
-        <v>1</v>
-      </c>
-      <c r="M78" s="75">
-        <v>1</v>
-      </c>
-      <c r="N78" s="75">
-        <v>1</v>
-      </c>
-      <c r="O78" s="75"/>
-      <c r="P78" s="77">
-        <v>1</v>
-      </c>
-      <c r="Q78" s="73">
-        <v>1</v>
-      </c>
-      <c r="R78" s="75">
-        <v>1</v>
-      </c>
-      <c r="S78" s="75">
-        <v>1</v>
-      </c>
-      <c r="T78" s="75"/>
-      <c r="U78" s="67">
-        <f>SUM(R78:T78)</f>
-        <v>2</v>
-      </c>
-      <c r="V78" s="14"/>
-      <c r="W78" s="3"/>
-      <c r="X78"/>
+      <c r="V78" s="31"/>
+      <c r="X78" s="31"/>
       <c r="Y78" s="31"/>
-      <c r="Z78"/>
-      <c r="AA78" s="31"/>
-      <c r="AB78" s="31"/>
-      <c r="AC78" s="31"/>
-      <c r="AD78" s="31"/>
+      <c r="Z78" s="31"/>
     </row>
     <row r="79" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="10"/>
       <c r="B79" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C79" s="22"/>
       <c r="D79" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E79" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F79" s="13">
-        <f>CEILING(D79,W$22+1)</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
       <c r="J79" s="13"/>
-      <c r="K79" s="21" t="s">
-        <v>109</v>
-      </c>
+      <c r="K79" s="21"/>
       <c r="L79" s="32">
         <v>1</v>
       </c>
@@ -7203,9 +7192,7 @@
       <c r="N79" s="75">
         <v>1</v>
       </c>
-      <c r="O79" s="75">
-        <v>1</v>
-      </c>
+      <c r="O79" s="75"/>
       <c r="P79" s="77">
         <v>1</v>
       </c>
@@ -7215,223 +7202,258 @@
       <c r="R79" s="75">
         <v>1</v>
       </c>
-      <c r="S79" s="75"/>
+      <c r="S79" s="75">
+        <v>1</v>
+      </c>
       <c r="T79" s="75"/>
       <c r="U79" s="67">
-        <f>SUM(R79:T79)</f>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="V79" s="14"/>
       <c r="W79" s="3"/>
-      <c r="X79" s="31"/>
+      <c r="X79"/>
       <c r="Y79" s="31"/>
-      <c r="Z79" s="31"/>
+      <c r="Z79"/>
       <c r="AA79" s="31"/>
       <c r="AB79" s="31"/>
       <c r="AC79" s="31"/>
       <c r="AD79" s="31"/>
     </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="10"/>
       <c r="B80" s="22" t="s">
-        <v>232</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="C80" s="22"/>
       <c r="D80" s="13">
         <v>1</v>
       </c>
       <c r="E80" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F80" s="13">
-        <f>CEILING(D80,W$22+1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="13"/>
       <c r="K80" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="L80" s="75"/>
+        <v>109</v>
+      </c>
+      <c r="L80" s="32">
+        <v>1</v>
+      </c>
+      <c r="M80" s="75">
+        <v>1</v>
+      </c>
+      <c r="N80" s="75">
+        <v>1</v>
+      </c>
+      <c r="O80" s="75">
+        <v>1</v>
+      </c>
       <c r="P80" s="77">
         <v>1</v>
       </c>
-      <c r="Q80" s="73"/>
+      <c r="Q80" s="73">
+        <v>1</v>
+      </c>
       <c r="R80" s="75">
         <v>1</v>
       </c>
+      <c r="S80" s="75"/>
+      <c r="T80" s="75"/>
       <c r="U80" s="67">
-        <f>SUM(R80:T80)</f>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="V80" s="14"/>
+      <c r="W80" s="3"/>
+      <c r="X80" s="31"/>
+      <c r="Y80" s="31"/>
+      <c r="Z80" s="31"/>
+      <c r="AA80" s="31"/>
+      <c r="AB80" s="31"/>
+      <c r="AC80" s="31"/>
+      <c r="AD80" s="31"/>
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B81" s="22" t="s">
-        <v>152</v>
+        <v>229</v>
       </c>
       <c r="D81" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E81" s="13">
         <v>1</v>
       </c>
       <c r="F81" s="13">
-        <f>CEILING(D81,W$22+1)</f>
-        <v>4</v>
-      </c>
-      <c r="K81" s="21"/>
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="K81" s="21" t="s">
+        <v>230</v>
+      </c>
       <c r="L81" s="75"/>
-      <c r="P81" s="77"/>
-      <c r="Q81" s="75"/>
+      <c r="P81" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q81" s="73"/>
+      <c r="R81" s="75">
+        <v>1</v>
+      </c>
       <c r="U81" s="67">
-        <f>SUM(R81:T81)</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="V81" s="14"/>
-      <c r="AA81" s="6"/>
-      <c r="AB81" s="6"/>
-      <c r="AC81" s="6"/>
-      <c r="AD81" s="6"/>
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B82" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D82" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E82" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82" s="13">
-        <f>CEILING(D82,W$22+1)</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="K82" s="21"/>
       <c r="L82" s="75"/>
       <c r="P82" s="77"/>
       <c r="Q82" s="75"/>
       <c r="U82" s="67">
-        <f>SUM(R82:T82)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V82" s="14"/>
-    </row>
-    <row r="83" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="10"/>
+      <c r="AA82" s="6"/>
+      <c r="AB82" s="6"/>
+      <c r="AC82" s="6"/>
+      <c r="AD82" s="6"/>
+    </row>
+    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B83" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C83" s="22"/>
+        <v>153</v>
+      </c>
       <c r="D83" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E83" s="13">
         <v>0</v>
       </c>
       <c r="F83" s="13">
-        <f>CEILING(D83,W$22+1)</f>
-        <v>4</v>
-      </c>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
       <c r="K83" s="21"/>
       <c r="L83" s="75"/>
-      <c r="M83" s="75"/>
-      <c r="N83" s="75"/>
-      <c r="O83" s="75"/>
       <c r="P83" s="77"/>
       <c r="Q83" s="75"/>
-      <c r="R83" s="75"/>
-      <c r="S83" s="75"/>
-      <c r="T83" s="75"/>
       <c r="U83" s="67">
-        <f>SUM(R83:T83)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V83" s="14"/>
-      <c r="W83" s="3"/>
-      <c r="X83"/>
-      <c r="Y83"/>
-      <c r="Z83"/>
-      <c r="AA83" s="6"/>
-      <c r="AB83" s="6"/>
-      <c r="AC83" s="6"/>
-      <c r="AD83" s="6"/>
-    </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B84" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="C84" s="23"/>
-      <c r="D84" s="26">
-        <v>1</v>
-      </c>
-      <c r="E84" s="26">
-        <v>0</v>
-      </c>
-      <c r="F84" s="26">
-        <f>CEILING(D84,W$22+1)</f>
+    </row>
+    <row r="84" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="10"/>
+      <c r="B84" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" s="22"/>
+      <c r="D84" s="13">
+        <v>4</v>
+      </c>
+      <c r="E84" s="13">
+        <v>0</v>
+      </c>
+      <c r="F84" s="13">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="21"/>
+      <c r="L84" s="75"/>
+      <c r="M84" s="75"/>
+      <c r="N84" s="75"/>
+      <c r="O84" s="75"/>
+      <c r="P84" s="77"/>
+      <c r="Q84" s="75"/>
+      <c r="R84" s="75"/>
+      <c r="S84" s="75"/>
+      <c r="T84" s="75"/>
+      <c r="U84" s="67">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V84" s="14"/>
+      <c r="W84" s="3"/>
+      <c r="X84"/>
+      <c r="Y84"/>
+      <c r="Z84"/>
+      <c r="AA84" s="6"/>
+      <c r="AB84" s="6"/>
+      <c r="AC84" s="6"/>
+      <c r="AD84" s="6"/>
+    </row>
+    <row r="85" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B85" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C85" s="23"/>
+      <c r="D85" s="26">
+        <v>1</v>
+      </c>
+      <c r="E85" s="26">
+        <v>0</v>
+      </c>
+      <c r="F85" s="26">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G84" s="26"/>
-      <c r="H84" s="26"/>
-      <c r="I84" s="26"/>
-      <c r="J84" s="26"/>
-      <c r="K84" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="L84" s="35"/>
-      <c r="M84" s="78"/>
-      <c r="N84" s="78">
-        <v>1</v>
-      </c>
-      <c r="O84" s="78">
-        <v>1</v>
-      </c>
-      <c r="P84" s="78"/>
-      <c r="Q84" s="35">
-        <v>1</v>
-      </c>
-      <c r="R84" s="78"/>
-      <c r="S84" s="78"/>
-      <c r="T84" s="78"/>
-      <c r="U84" s="81">
-        <f>SUM(R84:T84)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="11"/>
-      <c r="X85" s="31"/>
-      <c r="Y85" s="31"/>
-      <c r="Z85" s="31"/>
-      <c r="AA85" s="6"/>
-      <c r="AB85" s="6"/>
-      <c r="AC85" s="6"/>
-      <c r="AD85" s="6"/>
-    </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="K86" s="82"/>
-      <c r="L86" s="63"/>
-      <c r="M86" s="63"/>
-      <c r="N86" s="63"/>
-      <c r="O86" s="60" t="s">
-        <v>161</v>
-      </c>
-      <c r="P86" s="61"/>
-      <c r="Q86" s="61">
-        <f t="array" ref="Q86">SUM($F2:$F84*(Q2:Q84&gt;=0.9)*($U2:$U84&gt;=$W$12))</f>
-        <v>126</v>
-      </c>
-      <c r="R86" s="61">
-        <f t="array" ref="R86">SUM($F2:$F84*(R2:R84&gt;=0.9)*($U2:$U84&gt;=$W$12))</f>
-        <v>168</v>
-      </c>
-      <c r="S86" s="61">
-        <f t="array" ref="S86">SUM($F2:$F84*(S2:S84&gt;=0.9)*($U2:$U84&gt;=$W$12))</f>
-        <v>152</v>
-      </c>
-      <c r="T86" s="63"/>
+      <c r="G85" s="26"/>
+      <c r="H85" s="26"/>
+      <c r="I85" s="26"/>
+      <c r="J85" s="26"/>
+      <c r="K85" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="L85" s="35"/>
+      <c r="M85" s="78"/>
+      <c r="N85" s="78">
+        <v>1</v>
+      </c>
+      <c r="O85" s="78">
+        <v>1</v>
+      </c>
+      <c r="P85" s="78"/>
+      <c r="Q85" s="35">
+        <v>1</v>
+      </c>
+      <c r="R85" s="78"/>
+      <c r="S85" s="78"/>
+      <c r="T85" s="78"/>
+      <c r="U85" s="81">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="11"/>
+      <c r="X86" s="31"/>
+      <c r="Y86" s="31"/>
+      <c r="Z86" s="31"/>
       <c r="AA86" s="6"/>
       <c r="AB86" s="6"/>
       <c r="AC86" s="6"/>
@@ -7442,23 +7464,27 @@
       <c r="L87" s="63"/>
       <c r="M87" s="63"/>
       <c r="N87" s="63"/>
-      <c r="O87" s="62" t="s">
-        <v>163</v>
-      </c>
-      <c r="P87" s="63"/>
-      <c r="Q87" s="63">
-        <f t="array" ref="Q87">SUM($F2:$F84*Q2:Q84*($U2:$U84&gt;=$W$12))</f>
-        <v>128</v>
-      </c>
-      <c r="R87" s="63">
-        <f t="array" ref="R87">SUM($F2:$F84*R2:R84*($U2:$U84&gt;=$W$12))</f>
-        <v>170</v>
-      </c>
-      <c r="S87" s="63">
-        <f t="array" ref="S87">SUM($F2:$F84*S2:S84*($U2:$U84&gt;=$W$12))</f>
-        <v>152.4</v>
+      <c r="O87" s="60" t="s">
+        <v>161</v>
+      </c>
+      <c r="P87" s="61"/>
+      <c r="Q87" s="61">
+        <f t="array" ref="Q87">SUM($F2:$F85*(Q2:Q85&gt;=0.9)*($U2:$U85&gt;=$W$12))</f>
+        <v>148</v>
+      </c>
+      <c r="R87" s="61">
+        <f t="array" ref="R87">SUM($F2:$F85*(R2:R85&gt;=0.9)*($U2:$U85&gt;=$W$12))</f>
+        <v>168</v>
+      </c>
+      <c r="S87" s="61">
+        <f t="array" ref="S87">SUM($F2:$F85*(S2:S85&gt;=0.9)*($U2:$U85&gt;=$W$12))</f>
+        <v>152</v>
       </c>
       <c r="T87" s="63"/>
+      <c r="AA87" s="6"/>
+      <c r="AB87" s="6"/>
+      <c r="AC87" s="6"/>
+      <c r="AD87" s="6"/>
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.3">
       <c r="K88" s="82"/>
@@ -7466,20 +7492,20 @@
       <c r="M88" s="63"/>
       <c r="N88" s="63"/>
       <c r="O88" s="62" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="P88" s="63"/>
       <c r="Q88" s="63">
-        <f t="array" ref="Q88">SUM($F$2:$F$84*(Q$2:Q$84&gt;=0.1)*($U$2:$U$84&gt;=$W$12))</f>
-        <v>130</v>
+        <f t="array" ref="Q88">SUM($F2:$F85*Q2:Q85*($U2:$U85&gt;=$W$12))</f>
+        <v>150</v>
       </c>
       <c r="R88" s="63">
-        <f t="array" ref="R88">SUM($F$2:$F$84*(R$2:R$84&gt;=0.1)*($U$2:$U$84&gt;=$W$12))</f>
-        <v>172</v>
+        <f t="array" ref="R88">SUM($F2:$F85*R2:R85*($U2:$U85&gt;=$W$12))</f>
+        <v>170</v>
       </c>
       <c r="S88" s="63">
-        <f t="array" ref="S88">SUM($F$2:$F$84*(S$2:S$84&gt;=0.1)*($U$2:$U$84&gt;=$W$12))</f>
-        <v>156</v>
+        <f t="array" ref="S88">SUM($F2:$F85*S2:S85*($U2:$U85&gt;=$W$12))</f>
+        <v>152.4</v>
       </c>
       <c r="T88" s="63"/>
     </row>
@@ -7489,134 +7515,157 @@
       <c r="M89" s="63"/>
       <c r="N89" s="63"/>
       <c r="O89" s="62" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="P89" s="63"/>
       <c r="Q89" s="63">
-        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>222</v>
+        <f t="array" ref="Q89">SUM($F$2:$F$85*(Q$2:Q$85&gt;=0.1)*($U$2:$U$85&gt;=$W$12))</f>
+        <v>152</v>
       </c>
       <c r="R89" s="63">
-        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>222</v>
+        <f t="array" ref="R89">SUM($F$2:$F$85*(R$2:R$85&gt;=0.1)*($U$2:$U$85&gt;=$W$12))</f>
+        <v>172</v>
       </c>
       <c r="S89" s="63">
-        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>222</v>
+        <f t="array" ref="S89">SUM($F$2:$F$85*(S$2:S$85&gt;=0.1)*($U$2:$U$85&gt;=$W$12))</f>
+        <v>156</v>
       </c>
       <c r="T89" s="63"/>
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.3">
       <c r="K90" s="82"/>
-      <c r="L90" s="64"/>
-      <c r="M90" s="64"/>
-      <c r="N90" s="64"/>
+      <c r="L90" s="63"/>
+      <c r="M90" s="63"/>
+      <c r="N90" s="63"/>
       <c r="O90" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="P90" s="63"/>
+      <c r="Q90" s="63">
+        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
+        <v>244</v>
+      </c>
+      <c r="R90" s="63">
+        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
+        <v>244</v>
+      </c>
+      <c r="S90" s="63">
+        <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
+        <v>244</v>
+      </c>
+      <c r="T90" s="63"/>
+    </row>
+    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="K91" s="82"/>
+      <c r="L91" s="64"/>
+      <c r="M91" s="64"/>
+      <c r="N91" s="64"/>
+      <c r="O91" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="P90" s="64"/>
-      <c r="Q90" s="64">
-        <f>Q87/Q89</f>
-        <v>0.57657657657657657</v>
-      </c>
-      <c r="R90" s="64">
-        <f t="shared" ref="R90:S90" si="1">R87/R89</f>
-        <v>0.76576576576576572</v>
-      </c>
-      <c r="S90" s="64">
-        <f t="shared" si="1"/>
-        <v>0.68648648648648647</v>
-      </c>
-      <c r="T90" s="64"/>
-      <c r="Z90" s="31"/>
-    </row>
-    <row r="91" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D91" s="31"/>
-      <c r="K91" s="82"/>
-      <c r="L91" s="63"/>
-      <c r="M91" s="63"/>
-      <c r="N91" s="63"/>
-      <c r="O91" s="65" t="s">
+      <c r="P91" s="64"/>
+      <c r="Q91" s="64">
+        <f>Q88/Q90</f>
+        <v>0.61475409836065575</v>
+      </c>
+      <c r="R91" s="64">
+        <f t="shared" ref="R91:S91" si="6">R88/R90</f>
+        <v>0.69672131147540983</v>
+      </c>
+      <c r="S91" s="64">
+        <f t="shared" si="6"/>
+        <v>0.62459016393442623</v>
+      </c>
+      <c r="T91" s="64"/>
+      <c r="Z91" s="31"/>
+    </row>
+    <row r="92" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D92" s="31"/>
+      <c r="K92" s="82"/>
+      <c r="L92" s="63"/>
+      <c r="M92" s="63"/>
+      <c r="N92" s="63"/>
+      <c r="O92" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="P91" s="66"/>
-      <c r="Q91" s="66">
-        <f t="array" ref="Q91">SUM($F2:$F84*Q2:Q84*($U2:$U84&lt;$W$12))</f>
-        <v>37</v>
-      </c>
-      <c r="R91" s="66">
-        <f t="array" ref="R91">SUM($F2:$F84*R2:R84*($U2:$U84&lt;$W$12))</f>
+      <c r="P92" s="66"/>
+      <c r="Q92" s="66">
+        <f t="array" ref="Q92">SUM($F2:$F85*Q2:Q85*($U2:$U85&lt;$W$12))</f>
+        <v>15</v>
+      </c>
+      <c r="R92" s="66">
+        <f t="array" ref="R92">SUM($F2:$F85*R2:R85*($U2:$U85&lt;$W$12))</f>
         <v>3</v>
       </c>
-      <c r="S91" s="66">
-        <f t="array" ref="S91">SUM($F2:$F84*S2:S84*($U2:$U84&lt;$W$12))</f>
-        <v>0</v>
-      </c>
-      <c r="T91" s="63"/>
-    </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="D92" s="31"/>
-    </row>
-    <row r="93" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="10"/>
-      <c r="B93" s="22"/>
-      <c r="C93" s="22"/>
-      <c r="E93" s="13"/>
-      <c r="F93" s="13"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
-      <c r="K93" s="19"/>
-      <c r="L93" s="2"/>
-      <c r="M93" s="75"/>
-      <c r="N93" s="75"/>
-      <c r="O93" s="75"/>
-      <c r="P93" s="75"/>
-      <c r="Q93" s="2"/>
-      <c r="R93" s="75"/>
-      <c r="S93" s="75"/>
-      <c r="T93" s="75"/>
-      <c r="U93" s="3"/>
-      <c r="V93" s="3"/>
-      <c r="W93" s="3"/>
-      <c r="X93"/>
-      <c r="Y93"/>
-      <c r="Z93"/>
-      <c r="AA93"/>
-      <c r="AB93"/>
-      <c r="AC93"/>
-      <c r="AD93"/>
-    </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="D94" s="31"/>
-    </row>
-    <row r="99" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA99" s="6"/>
-      <c r="AB99" s="6"/>
-      <c r="AC99" s="6"/>
-      <c r="AD99" s="6"/>
-    </row>
-    <row r="103" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA103" s="6"/>
-      <c r="AB103" s="6"/>
-      <c r="AC103" s="6"/>
-      <c r="AD103" s="6"/>
-    </row>
-    <row r="108" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA108" s="6"/>
-      <c r="AB108" s="6"/>
-      <c r="AC108" s="6"/>
-      <c r="AD108" s="6"/>
-    </row>
-    <row r="121" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA121" s="31"/>
-      <c r="AB121" s="31"/>
-      <c r="AC121" s="31"/>
-      <c r="AD121" s="31"/>
+      <c r="S92" s="66">
+        <f t="array" ref="S92">SUM($F2:$F85*S2:S85*($U2:$U85&lt;$W$12))</f>
+        <v>0</v>
+      </c>
+      <c r="T92" s="63"/>
+    </row>
+    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="D93" s="31"/>
+    </row>
+    <row r="94" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="10"/>
+      <c r="B94" s="22"/>
+      <c r="C94" s="22"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="13"/>
+      <c r="K94" s="19"/>
+      <c r="L94" s="2"/>
+      <c r="M94" s="75"/>
+      <c r="N94" s="75"/>
+      <c r="O94" s="75"/>
+      <c r="P94" s="75"/>
+      <c r="Q94" s="2"/>
+      <c r="R94" s="75"/>
+      <c r="S94" s="75"/>
+      <c r="T94" s="75"/>
+      <c r="U94" s="3"/>
+      <c r="V94" s="3"/>
+      <c r="W94" s="3"/>
+      <c r="X94"/>
+      <c r="Y94"/>
+      <c r="Z94"/>
+      <c r="AA94"/>
+      <c r="AB94"/>
+      <c r="AC94"/>
+      <c r="AD94"/>
+    </row>
+    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="D95" s="31"/>
+    </row>
+    <row r="100" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA100" s="6"/>
+      <c r="AB100" s="6"/>
+      <c r="AC100" s="6"/>
+      <c r="AD100" s="6"/>
+    </row>
+    <row r="104" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA104" s="6"/>
+      <c r="AB104" s="6"/>
+      <c r="AC104" s="6"/>
+      <c r="AD104" s="6"/>
+    </row>
+    <row r="109" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA109" s="6"/>
+      <c r="AB109" s="6"/>
+      <c r="AC109" s="6"/>
+      <c r="AD109" s="6"/>
+    </row>
+    <row r="122" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA122" s="31"/>
+      <c r="AB122" s="31"/>
+      <c r="AC122" s="31"/>
+      <c r="AD122" s="31"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U84">
+  <conditionalFormatting sqref="B2:U59 B61:U85 C60:U60">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
       <formula>$U2&gt;=(0.5+$W$12)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixed typo, minor update to spreadsheet
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2021spring.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2021spring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Desktop\github\132\StudentGuideModule2\what_labs_to_include\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747CCA84-CDAC-4184-B909-705275FD06F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08723872-15D6-4D2C-88B6-37F9B8D97D96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18780" yWindow="5136" windowWidth="26616" windowHeight="15936" tabRatio="541" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2922,8 +2922,8 @@
   <dimension ref="A1:AD122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K61" sqref="K61"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4399,15 +4399,15 @@
         <v>0</v>
       </c>
       <c r="X26" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W26,F$2:F$86)</f>
+        <f t="shared" ref="X26:X34" si="2">SUMIF(U$2:U$86,"&gt;=" &amp; W26,F$2:F$86)</f>
         <v>370</v>
       </c>
       <c r="Y26" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W26,E$2:E$86)</f>
+        <f t="shared" ref="Y26:Y34" si="3">SUMIF(U$2:U$86,"&gt;=" &amp; W26,E$2:E$86)</f>
         <v>29</v>
       </c>
       <c r="Z26" s="8">
-        <f t="shared" ref="Z26:Z34" si="2">($Y$17 + $Y$15*X26+$Y$16*Y26)*(1+Y$18+Y$19)</f>
+        <f t="shared" ref="Z26:Z34" si="4">($Y$17 + $Y$15*X26+$Y$16*Y26)*(1+Y$18+Y$19)</f>
         <v>39.26</v>
       </c>
       <c r="AA26" s="31"/>
@@ -4452,11 +4452,11 @@
         <v>0.5</v>
       </c>
       <c r="X27" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W27,F$2:F$86)</f>
+        <f t="shared" si="2"/>
         <v>270</v>
       </c>
       <c r="Y27" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W27,E$2:E$86)</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="Z27" s="8">
@@ -4528,15 +4528,15 @@
         <v>1</v>
       </c>
       <c r="X28" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W28,F$2:F$86)</f>
+        <f t="shared" si="2"/>
         <v>244</v>
       </c>
       <c r="Y28" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W28,E$2:E$86)</f>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="Z28" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>28.340000000000003</v>
       </c>
     </row>
@@ -4599,15 +4599,15 @@
         <v>1.5</v>
       </c>
       <c r="X29" s="29">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W29,F$2:F$86)</f>
+        <f t="shared" si="2"/>
         <v>172</v>
       </c>
       <c r="Y29" s="29">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W29,E$2:E$86)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="Z29" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>21.32</v>
       </c>
       <c r="AA29" s="31"/>
@@ -4655,15 +4655,15 @@
         <v>2</v>
       </c>
       <c r="X30" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W30,F$2:F$86)</f>
+        <f t="shared" si="2"/>
         <v>166</v>
       </c>
       <c r="Y30" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W30,E$2:E$86)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="Z30" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20.930000000000003</v>
       </c>
     </row>
@@ -4705,15 +4705,15 @@
         <v>2.5</v>
       </c>
       <c r="X31" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W31,F$2:F$86)</f>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="Y31" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W31,E$2:E$86)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="Z31" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10.530000000000003</v>
       </c>
       <c r="AA31" s="31"/>
@@ -4770,15 +4770,15 @@
         <v>3</v>
       </c>
       <c r="X32" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W32,F$2:F$86)</f>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="Y32" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W32,E$2:E$86)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="Z32" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10.530000000000003</v>
       </c>
     </row>
@@ -4849,15 +4849,15 @@
         <v>3.5</v>
       </c>
       <c r="X33" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W33,F$2:F$86)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Y33" s="6">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W33,E$2:E$86)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Z33" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.2</v>
       </c>
       <c r="AA33"/>
@@ -4879,7 +4879,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="13">
-        <f t="shared" ref="F34:F66" si="3">CEILING(D34,W$22+1)</f>
+        <f t="shared" ref="F34:F66" si="5">CEILING(D34,W$22+1)</f>
         <v>2</v>
       </c>
       <c r="J34" s="13">
@@ -4921,15 +4921,15 @@
         <v>4</v>
       </c>
       <c r="X34" s="45">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W34,F$2:F$86)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Y34" s="45">
-        <f>SUMIF(U$2:U$86,"&gt;=" &amp; W34,E$2:E$86)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Z34" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.2</v>
       </c>
     </row>
@@ -4948,7 +4948,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G35" s="13">
@@ -5018,7 +5018,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G36" s="13">
@@ -5064,7 +5064,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="H37" s="13">
@@ -5117,7 +5117,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="J38" s="13">
@@ -5165,7 +5165,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="J39" s="13">
@@ -5213,7 +5213,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G40" s="13">
@@ -5280,7 +5280,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G41" s="12" t="s">
@@ -5346,7 +5346,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G42" s="13">
@@ -5413,7 +5413,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="K43" s="21" t="s">
@@ -5444,7 +5444,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="H44" s="13">
@@ -5496,7 +5496,7 @@
         <v>2</v>
       </c>
       <c r="F45" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G45" s="13" t="s">
@@ -5556,7 +5556,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G46" s="12" t="s">
@@ -5616,7 +5616,7 @@
         <v>2</v>
       </c>
       <c r="F47" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="K47" s="21" t="s">
@@ -5661,7 +5661,7 @@
         <v>3</v>
       </c>
       <c r="F48" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G48" s="13" t="s">
@@ -5726,7 +5726,7 @@
         <v>4</v>
       </c>
       <c r="F49" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G49" s="13"/>
@@ -5776,7 +5776,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G50" s="13">
@@ -5834,7 +5834,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G51" s="13">
@@ -5887,7 +5887,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G52" s="12">
@@ -5946,7 +5946,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G53" s="13">
@@ -5998,7 +5998,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G54" s="12"/>
@@ -6057,7 +6057,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G55" s="13">
@@ -6114,7 +6114,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G56" s="13">
@@ -6166,7 +6166,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G57" s="13">
@@ -6204,7 +6204,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G58" s="13">
@@ -6262,7 +6262,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G59" s="13">
@@ -6322,7 +6322,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G60" s="13"/>
@@ -6364,7 +6364,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G61" s="13">
@@ -6420,7 +6420,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G62" s="13"/>
@@ -6459,7 +6459,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="H63" s="13">
@@ -6517,7 +6517,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="J64" s="13">
@@ -6557,7 +6557,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="J65" s="13">
@@ -6602,7 +6602,7 @@
         <v>2</v>
       </c>
       <c r="F66" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="G66" s="13">
@@ -6641,7 +6641,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="13">
-        <f t="shared" ref="F67:F85" si="4">CEILING(D67,W$22+1)</f>
+        <f t="shared" ref="F67:F85" si="6">CEILING(D67,W$22+1)</f>
         <v>8</v>
       </c>
       <c r="G67" s="13">
@@ -6658,7 +6658,7 @@
         <v>1</v>
       </c>
       <c r="U67" s="67">
-        <f t="shared" ref="U67:U85" si="5">SUM(Q67:T67)</f>
+        <f t="shared" ref="U67:U85" si="7">SUM(Q67:T67)</f>
         <v>1</v>
       </c>
       <c r="V67" s="31"/>
@@ -6679,7 +6679,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="J68" s="13">
@@ -6703,7 +6703,7 @@
       <c r="Q68" s="32"/>
       <c r="T68" s="78"/>
       <c r="U68" s="81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V68" s="31"/>
@@ -6726,7 +6726,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G69" s="12">
@@ -6762,7 +6762,7 @@
       </c>
       <c r="T69" s="77"/>
       <c r="U69" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="V69" s="31"/>
@@ -6789,7 +6789,7 @@
         <v>2</v>
       </c>
       <c r="F70" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="G70" s="13">
@@ -6803,7 +6803,7 @@
         <v>1</v>
       </c>
       <c r="U70" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V70" s="31"/>
@@ -6822,7 +6822,7 @@
         <v>2</v>
       </c>
       <c r="F71" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="G71" s="13">
@@ -6833,7 +6833,7 @@
       <c r="P71" s="77"/>
       <c r="Q71" s="31"/>
       <c r="U71" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V71" s="31"/>
@@ -6853,7 +6853,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="G72" s="26">
@@ -6877,7 +6877,7 @@
       <c r="S72" s="78"/>
       <c r="T72" s="78"/>
       <c r="U72" s="81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V72" s="31"/>
@@ -6901,7 +6901,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G73" s="13">
@@ -6921,7 +6921,7 @@
       <c r="S73" s="75"/>
       <c r="T73" s="75"/>
       <c r="U73" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V73" s="31"/>
@@ -6948,7 +6948,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G74" s="13">
@@ -6959,7 +6959,7 @@
       <c r="P74" s="77"/>
       <c r="Q74" s="32"/>
       <c r="U74" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V74" s="31"/>
@@ -6983,7 +6983,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G75" s="13"/>
@@ -7003,7 +7003,7 @@
       <c r="S75" s="75"/>
       <c r="T75" s="78"/>
       <c r="U75" s="81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W75" s="3"/>
@@ -7030,7 +7030,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G76" s="12"/>
@@ -7060,7 +7060,7 @@
       <c r="S76" s="76"/>
       <c r="T76" s="77"/>
       <c r="U76" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V76" s="31"/>
@@ -7078,7 +7078,7 @@
         <v>1</v>
       </c>
       <c r="F77" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G77" s="13"/>
@@ -7112,7 +7112,7 @@
       </c>
       <c r="T77" s="77"/>
       <c r="U77" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="W77" s="3"/>
@@ -7130,7 +7130,7 @@
         <v>1</v>
       </c>
       <c r="F78" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K78" s="21" t="s">
@@ -7154,7 +7154,7 @@
         <v>2</v>
       </c>
       <c r="U78" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="V78" s="31"/>
@@ -7175,7 +7175,7 @@
         <v>3</v>
       </c>
       <c r="F79" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G79" s="13"/>
@@ -7207,7 +7207,7 @@
       </c>
       <c r="T79" s="75"/>
       <c r="U79" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="V79" s="14"/>
@@ -7233,7 +7233,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G80" s="13"/>
@@ -7267,7 +7267,7 @@
       <c r="S80" s="75"/>
       <c r="T80" s="75"/>
       <c r="U80" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="V80" s="14"/>
@@ -7291,7 +7291,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K81" s="21" t="s">
@@ -7306,7 +7306,7 @@
         <v>1</v>
       </c>
       <c r="U81" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V81" s="14"/>
@@ -7322,7 +7322,7 @@
         <v>1</v>
       </c>
       <c r="F82" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="K82" s="21"/>
@@ -7330,7 +7330,7 @@
       <c r="P82" s="77"/>
       <c r="Q82" s="75"/>
       <c r="U82" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V82" s="14"/>
@@ -7350,7 +7350,7 @@
         <v>0</v>
       </c>
       <c r="F83" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K83" s="21"/>
@@ -7358,7 +7358,7 @@
       <c r="P83" s="77"/>
       <c r="Q83" s="75"/>
       <c r="U83" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V83" s="14"/>
@@ -7376,7 +7376,7 @@
         <v>0</v>
       </c>
       <c r="F84" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G84" s="13"/>
@@ -7394,7 +7394,7 @@
       <c r="S84" s="75"/>
       <c r="T84" s="75"/>
       <c r="U84" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V84" s="14"/>
@@ -7419,7 +7419,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G85" s="26"/>
@@ -7445,7 +7445,7 @@
       <c r="S85" s="78"/>
       <c r="T85" s="78"/>
       <c r="U85" s="81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7569,11 +7569,11 @@
         <v>0.61475409836065575</v>
       </c>
       <c r="R91" s="64">
-        <f t="shared" ref="R91:S91" si="6">R88/R90</f>
+        <f t="shared" ref="R91:S91" si="8">R88/R90</f>
         <v>0.69672131147540983</v>
       </c>
       <c r="S91" s="64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.62459016393442623</v>
       </c>
       <c r="T91" s="64"/>

</xml_diff>

<commit_message>
Last changes for spring 2021
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2021spring.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2021spring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Desktop\github\132\StudentGuideModule2\what_labs_to_include\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498BE80D-8AF8-420F-BFD4-25A6C1D2B984}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD04DDB-038A-4B9D-A759-3D3390CF4969}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18780" yWindow="5136" windowWidth="26616" windowHeight="15936" tabRatio="541" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2931,8 +2931,8 @@
   <dimension ref="A1:Z122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4342,7 +4342,7 @@
       </c>
       <c r="T27" s="6">
         <f t="shared" si="2"/>
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="U27" s="6">
         <f t="shared" si="3"/>
@@ -4350,7 +4350,7 @@
       </c>
       <c r="V27" s="8">
         <f>($U$17 + $U$15*T27+$U$16*U27)*(1+U$18+U$19)</f>
-        <v>32.500000000000007</v>
+        <v>32.11</v>
       </c>
       <c r="W27" s="31"/>
       <c r="X27" s="31"/>
@@ -4410,15 +4410,15 @@
       </c>
       <c r="T28" s="6">
         <f t="shared" si="2"/>
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="U28" s="6">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="V28" s="8">
         <f t="shared" si="4"/>
-        <v>31.46</v>
+        <v>28.990000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
@@ -4634,15 +4634,15 @@
       </c>
       <c r="T32" s="6">
         <f t="shared" si="2"/>
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="U32" s="6">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="V32" s="8">
         <f t="shared" si="4"/>
-        <v>13.91</v>
+        <v>10.790000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -5348,14 +5348,14 @@
         <v>1</v>
       </c>
       <c r="M46" s="33">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N46" s="76"/>
       <c r="O46" s="86"/>
       <c r="P46" s="77"/>
       <c r="Q46" s="67">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S46" s="3"/>
     </row>
@@ -5386,7 +5386,7 @@
       <c r="K47" s="77"/>
       <c r="L47" s="77"/>
       <c r="M47" s="77">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N47" s="77">
         <v>1</v>
@@ -5397,7 +5397,7 @@
       <c r="P47" s="77"/>
       <c r="Q47" s="67">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="R47" s="31"/>
       <c r="V47" s="6"/>
@@ -5443,14 +5443,14 @@
         <v>0.9</v>
       </c>
       <c r="M48" s="32">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N48" s="75"/>
       <c r="O48" s="84"/>
       <c r="P48" s="75"/>
       <c r="Q48" s="67">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S48" s="3"/>
       <c r="V48" s="6"/>
@@ -5486,7 +5486,7 @@
       <c r="K49" s="75"/>
       <c r="L49" s="77"/>
       <c r="M49" s="75">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N49" s="75">
         <v>1</v>
@@ -5497,7 +5497,7 @@
       <c r="P49" s="75"/>
       <c r="Q49" s="67">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="R49" s="31"/>
       <c r="S49" s="14"/>
@@ -6210,12 +6210,12 @@
         <v>1</v>
       </c>
       <c r="M65" s="32">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O65" s="83"/>
       <c r="Q65" s="67">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R65" s="31"/>
       <c r="W65" s="31"/>
@@ -7046,7 +7046,7 @@
       <c r="L87" s="61"/>
       <c r="M87" s="61">
         <f t="array" ref="M87">SUM($F2:$F85*(M2:M85&gt;=0.9)*($Q2:$Q85&gt;=$S$12))</f>
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="N87" s="61">
         <f t="array" ref="N87">SUM($F2:$F85*(N2:N85&gt;=0.9)*($Q2:$Q85&gt;=$S$12))</f>
@@ -7073,7 +7073,7 @@
       <c r="L88" s="63"/>
       <c r="M88" s="63">
         <f t="array" ref="M88">SUM($F2:$F85*M2:M85*($Q2:$Q85&gt;=$S$12))</f>
-        <v>142.4</v>
+        <v>136.4</v>
       </c>
       <c r="N88" s="63">
         <f t="array" ref="N88">SUM($F2:$F85*N2:N85*($Q2:$Q85&gt;=$S$12))</f>
@@ -7142,7 +7142,7 @@
       <c r="L91" s="64"/>
       <c r="M91" s="64">
         <f>M88/M90</f>
-        <v>0.81839080459770119</v>
+        <v>0.78390804597701158</v>
       </c>
       <c r="N91" s="64">
         <f t="shared" ref="N91:O91" si="8">N88/N90</f>
@@ -7167,7 +7167,7 @@
       <c r="L92" s="66"/>
       <c r="M92" s="66">
         <f t="array" ref="M92">SUM($F2:$F85*M2:M85*($Q2:$Q85&lt;$S$12))</f>
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="N92" s="66">
         <f t="array" ref="N92">SUM($F2:$F85*N2:N85*($Q2:$Q85&lt;$S$12))</f>

</xml_diff>